<commit_message>
HELCOM data processing enhancements:
- Added temperature and salinity callbacks for improved data handling.
- Cleaned and updated dbo_lab.xlsx to ensure data integrity and consistency.
</commit_message>
<xml_diff>
--- a/nbs/files/lut/dbo_lab.xlsx
+++ b/nbs/files/lut/dbo_lab.xlsx
@@ -1,16 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10911"/>
-  <workbookPr defaultThemeVersion="166925"/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/franckalbinet/pro/IAEA/MARIS/marisco/nbs/files/lut/"/>
-    </mc:Choice>
-  </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9DB7A838-65EA-9648-A0CF-FB05DEDE1A49}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="7" rupBuild="9303"/>
+  <workbookPr/>
   <bookViews>
-    <workbookView xWindow="4440" yWindow="2500" windowWidth="21600" windowHeight="12740" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="4440" yWindow="2505" windowWidth="21600" windowHeight="12735"/>
   </bookViews>
   <sheets>
     <sheet name="dbo_lab" sheetId="1" r:id="rId1"/>
@@ -39,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2142" uniqueCount="1610">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2143" uniqueCount="1610">
   <si>
     <t>lab_id</t>
   </si>
@@ -4875,7 +4869,7 @@
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -5235,33 +5229,33 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:N502"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="C1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A3" sqref="A3"/>
+      <selection pane="bottomLeft" activeCell="C2" sqref="C2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="9.1640625" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="1" width="14.1640625" customWidth="1"/>
-    <col min="2" max="2" width="13.5" customWidth="1"/>
-    <col min="3" max="3" width="136.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="29.5" customWidth="1"/>
-    <col min="6" max="6" width="27.5" customWidth="1"/>
+    <col min="1" max="1" width="14.140625" customWidth="1"/>
+    <col min="2" max="2" width="13.42578125" customWidth="1"/>
+    <col min="3" max="3" width="136.42578125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="29.42578125" customWidth="1"/>
+    <col min="6" max="6" width="27.42578125" customWidth="1"/>
     <col min="8" max="8" width="12" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="52.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="52.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -5296,15 +5290,18 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>-1</v>
       </c>
       <c r="B2" t="s">
         <v>1609</v>
       </c>
-    </row>
-    <row r="3" spans="1:14" x14ac:dyDescent="0.2">
+      <c r="C2" t="s">
+        <v>1609</v>
+      </c>
+    </row>
+    <row r="3" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>0</v>
       </c>
@@ -5319,7 +5316,7 @@
       </c>
       <c r="N3" s="6"/>
     </row>
-    <row r="4" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1</v>
       </c>
@@ -5343,7 +5340,7 @@
         <v>update lab set lab = 'International Atomic Energy Agency - Environment Laboratory (former Marine Environment Laboratory)', country = '' where lab_id = 1</v>
       </c>
     </row>
-    <row r="5" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>2</v>
       </c>
@@ -5364,7 +5361,7 @@
         <v>update lab set lab = 'Institute of Nuclear Physics - Academy of Sciences', country = '' where lab_id = 2</v>
       </c>
     </row>
-    <row r="6" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>3</v>
       </c>
@@ -5388,7 +5385,7 @@
         <v>update lab set lab = 'Institut des Sciences de la Mer et de l'Aménagement du Littoral', country = '' where lab_id = 3</v>
       </c>
     </row>
-    <row r="7" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>4</v>
       </c>
@@ -5415,7 +5412,7 @@
         <v>update lab set lab = 'Centre de Radioprotection et Sûreté - Lab. d'Environnement', country = '' where lab_id = 4</v>
       </c>
     </row>
-    <row r="8" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>5</v>
       </c>
@@ -5439,7 +5436,7 @@
         <v>update lab set lab = 'Central Mining Institute', country = '' where lab_id = 5</v>
       </c>
     </row>
-    <row r="9" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>6</v>
       </c>
@@ -5466,7 +5463,7 @@
         <v>update lab set lab = 'Atomic Energy Minerals Centre', country = '' where lab_id = 6</v>
       </c>
     </row>
-    <row r="10" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>7</v>
       </c>
@@ -5490,7 +5487,7 @@
         <v>update lab set lab = 'Australian Nuclear Science and Technology Organization - Environmental Services', country = '' where lab_id = 7</v>
       </c>
     </row>
-    <row r="11" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>8</v>
       </c>
@@ -5511,7 +5508,7 @@
         <v>update lab set lab = 'Australian Nuclear Science and Technology Organization', country = '' where lab_id = 8</v>
       </c>
     </row>
-    <row r="12" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>9</v>
       </c>
@@ -5532,7 +5529,7 @@
         <v>update lab set lab = 'Alligator Rivers Region Research Institute', country = '' where lab_id = 9</v>
       </c>
     </row>
-    <row r="13" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>10</v>
       </c>
@@ -5547,7 +5544,7 @@
         <v>update lab set lab = 'US Coast Guard', country = '' where lab_id = 10</v>
       </c>
     </row>
-    <row r="14" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>11</v>
       </c>
@@ -5568,7 +5565,7 @@
         <v>update lab set lab = 'Quality Control Officer - ANALABS', country = '' where lab_id = 11</v>
       </c>
     </row>
-    <row r="15" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>12</v>
       </c>
@@ -5589,7 +5586,7 @@
         <v>update lab set lab = 'Office of the Supervising Scientist', country = '' where lab_id = 12</v>
       </c>
     </row>
-    <row r="16" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A16">
         <v>13</v>
       </c>
@@ -5610,7 +5607,7 @@
         <v>update lab set lab = 'Atominstitut der Osterreichischen Universitäten', country = '' where lab_id = 13</v>
       </c>
     </row>
-    <row r="17" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A17">
         <v>14</v>
       </c>
@@ -5634,7 +5631,7 @@
         <v>update lab set lab = 'BALUF Wien', country = '' where lab_id = 14</v>
       </c>
     </row>
-    <row r="18" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>15</v>
       </c>
@@ -5655,7 +5652,7 @@
         <v>update lab set lab = 'BVFA Arsenal - Geotechnisches Institut Isotopengeophysik', country = '' where lab_id = 15</v>
       </c>
     </row>
-    <row r="19" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>16</v>
       </c>
@@ -5676,7 +5673,7 @@
         <v>update lab set lab = 'Federal Institute for Food Control and Research - Radiochemistry', country = '' where lab_id = 16</v>
       </c>
     </row>
-    <row r="20" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>17</v>
       </c>
@@ -5700,7 +5697,7 @@
         <v>update lab set lab = 'International Atomic Energy Agency - Seibersdorf Laboratory', country = '' where lab_id = 17</v>
       </c>
     </row>
-    <row r="21" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>18</v>
       </c>
@@ -5721,7 +5718,7 @@
         <v>update lab set lab = 'Institute of Physics', country = '' where lab_id = 18</v>
       </c>
     </row>
-    <row r="22" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>19</v>
       </c>
@@ -5742,7 +5739,7 @@
         <v>update lab set lab = 'National Focal Point - Environmental Protection Committee', country = '' where lab_id = 19</v>
       </c>
     </row>
-    <row r="23" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>20</v>
       </c>
@@ -5766,7 +5763,7 @@
         <v>update lab set lab = 'Inst. of Nuclear Science &amp; Technology - Atomic Energy Research Establishment', country = '' where lab_id = 20</v>
       </c>
     </row>
-    <row r="24" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A24">
         <v>21</v>
       </c>
@@ -5787,7 +5784,7 @@
         <v>update lab set lab = 'Laboratoire du C.E.N/S.C.K - Section de Spectrométrie Nucléaire', country = '' where lab_id = 21</v>
       </c>
     </row>
-    <row r="25" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A25">
         <v>22</v>
       </c>
@@ -5805,7 +5802,7 @@
         <v>update lab set lab = 'Lamont Doherty Geological Observatory', country = '' where lab_id = 22</v>
       </c>
     </row>
-    <row r="26" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A26">
         <v>23</v>
       </c>
@@ -5829,7 +5826,7 @@
         <v>update lab set lab = 'Universidad Mayor de San Andrés - Facultad de Ciencias Puras y Naturales', country = '' where lab_id = 23</v>
       </c>
     </row>
-    <row r="27" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>24</v>
       </c>
@@ -5853,7 +5850,7 @@
         <v>update lab set lab = 'Instituto Boliviano de Ciencias y Tecnologia Nuclear - PNUD', country = '' where lab_id = 24</v>
       </c>
     </row>
-    <row r="28" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>25</v>
       </c>
@@ -5871,7 +5868,7 @@
         <v>update lab set lab = 'National Swedish Environmental Protection, Coastal Research Lab', country = '' where lab_id = 25</v>
       </c>
     </row>
-    <row r="29" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>26</v>
       </c>
@@ -5889,7 +5886,7 @@
         <v>update lab set lab = 'Veterinary Faculty of the University of Sarajevo', country = '' where lab_id = 26</v>
       </c>
     </row>
-    <row r="30" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>27</v>
       </c>
@@ -5907,7 +5904,7 @@
         <v>update lab set lab = 'Inst for Experimental Meteorology', country = '' where lab_id = 27</v>
       </c>
     </row>
-    <row r="31" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>28</v>
       </c>
@@ -5931,7 +5928,7 @@
         <v>update lab set lab = 'Instituto de Pesquisas Energéticas e Nucleares', country = '' where lab_id = 28</v>
       </c>
     </row>
-    <row r="32" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>29</v>
       </c>
@@ -5955,7 +5952,7 @@
         <v>update lab set lab = 'Furnas Centrais Eletricas S.A. - CNAAA - Laboratorio de Radioecolog.', country = '' where lab_id = 29</v>
       </c>
     </row>
-    <row r="33" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A33">
         <v>30</v>
       </c>
@@ -5979,7 +5976,7 @@
         <v>update lab set lab = 'Furnas Centrais Eletricas S.A. - Depart. de Geracao de Angra.', country = '' where lab_id = 30</v>
       </c>
     </row>
-    <row r="34" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>31</v>
       </c>
@@ -6003,7 +6000,7 @@
         <v>update lab set lab = 'Instituto de Pesquisas Energéticas e Nucleares - Environmental Monitoring Division ', country = '' where lab_id = 31</v>
       </c>
     </row>
-    <row r="35" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>32</v>
       </c>
@@ -6021,7 +6018,7 @@
         <v>update lab set lab = 'Instituto de Radioprotecao e Dosimetria', country = '' where lab_id = 32</v>
       </c>
     </row>
-    <row r="36" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>33</v>
       </c>
@@ -6042,7 +6039,7 @@
         <v>update lab set lab = 'Institute of Nuclear Medicine Radiobiology &amp; Radiation Hygiene - Radiation Hygiene Research Division', country = '' where lab_id = 33</v>
       </c>
     </row>
-    <row r="37" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>34</v>
       </c>
@@ -6060,7 +6057,7 @@
         <v>update lab set lab = 'Atomic Energy of Canada Ltd. - Whiteshell Nuclear Research Establ.', country = '' where lab_id = 34</v>
       </c>
     </row>
-    <row r="38" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>35</v>
       </c>
@@ -6084,7 +6081,7 @@
         <v>update lab set lab = 'Senior Research Officer and Visiting Professor', country = '' where lab_id = 35</v>
       </c>
     </row>
-    <row r="39" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>36</v>
       </c>
@@ -6108,7 +6105,7 @@
         <v>update lab set lab = 'Environmental Radiation Hazards D. - Bureau of Radiation &amp; Med. Devices', country = '' where lab_id = 36</v>
       </c>
     </row>
-    <row r="40" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A40">
         <v>37</v>
       </c>
@@ -6135,7 +6132,7 @@
         <v>update lab set lab = 'Bedford Institute of Oceanography - Dept. of Fisheries and Oceans', country = '' where lab_id = 37</v>
       </c>
     </row>
-    <row r="41" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>38</v>
       </c>
@@ -6159,7 +6156,7 @@
         <v>update lab set lab = 'Atlantic Environ. Radiation Unit - Bedford Institute of Oceanography', country = '' where lab_id = 38</v>
       </c>
     </row>
-    <row r="42" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>39</v>
       </c>
@@ -6180,7 +6177,7 @@
         <v>update lab set lab = 'Ontario Ministry of Labour - Radiation Protection Service', country = '' where lab_id = 39</v>
       </c>
     </row>
-    <row r="43" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>40</v>
       </c>
@@ -6201,7 +6198,7 @@
         <v>update lab set lab = 'Fisheries and Oceans Canada - Freshwater Institute', country = '' where lab_id = 40</v>
       </c>
     </row>
-    <row r="44" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>41</v>
       </c>
@@ -6222,7 +6219,7 @@
         <v>update lab set lab = 'Ecole Polytechnique', country = '' where lab_id = 41</v>
       </c>
     </row>
-    <row r="45" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>42</v>
       </c>
@@ -6246,7 +6243,7 @@
         <v>update lab set lab = 'Direccion General del Territorio Maritimo y de Marina Mercante', country = '' where lab_id = 42</v>
       </c>
     </row>
-    <row r="46" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>43</v>
       </c>
@@ -6264,7 +6261,7 @@
         <v>update lab set lab = 'Third Institute of Oceanography - State Oceanic Administration', country = '' where lab_id = 43</v>
       </c>
     </row>
-    <row r="47" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A47">
         <v>44</v>
       </c>
@@ -6282,7 +6279,7 @@
         <v>update lab set lab = 'McMasters University', country = '' where lab_id = 44</v>
       </c>
     </row>
-    <row r="48" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A48">
         <v>45</v>
       </c>
@@ -6306,7 +6303,7 @@
         <v>update lab set lab = 'Institute of Radiation Medicine - Chinese Academy of Medical Sciences', country = '' where lab_id = 45</v>
       </c>
     </row>
-    <row r="49" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A49">
         <v>46</v>
       </c>
@@ -6324,7 +6321,7 @@
         <v>update lab set lab = 'Nanjing University - Department of GEO &amp; OCEAN Services', country = '' where lab_id = 46</v>
       </c>
     </row>
-    <row r="50" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A50">
         <v>47</v>
       </c>
@@ -6348,7 +6345,7 @@
         <v>update lab set lab = 'First Institute of Oceanography', country = '' where lab_id = 47</v>
       </c>
     </row>
-    <row r="51" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A51">
         <v>48</v>
       </c>
@@ -6369,7 +6366,7 @@
         <v>update lab set lab = 'Beijing Institute of Chemical Engineering and Metallurgy', country = '' where lab_id = 48</v>
       </c>
     </row>
-    <row r="52" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A52">
         <v>49</v>
       </c>
@@ -6390,7 +6387,7 @@
         <v>update lab set lab = 'AEA Technology - Winfrith Technology Centre', country = '' where lab_id = 49</v>
       </c>
     </row>
-    <row r="53" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A53">
         <v>50</v>
       </c>
@@ -6411,7 +6408,7 @@
         <v>update lab set lab = 'China Institute for Radiation Protection', country = '' where lab_id = 50</v>
       </c>
     </row>
-    <row r="54" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A54">
         <v>51</v>
       </c>
@@ -6432,7 +6429,7 @@
         <v>update lab set lab = 'China Institute of Atomic Energy', country = '' where lab_id = 51</v>
       </c>
     </row>
-    <row r="55" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A55">
         <v>52</v>
       </c>
@@ -6453,7 +6450,7 @@
         <v>update lab set lab = 'Institute of Oceanography and Fisheries', country = '' where lab_id = 52</v>
       </c>
     </row>
-    <row r="56" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A56">
         <v>53</v>
       </c>
@@ -6477,7 +6474,7 @@
         <v>update lab set lab = 'Inst. for Med. Res. &amp; Occ. Health - Department of Radiation Protection', country = '' where lab_id = 53</v>
       </c>
     </row>
-    <row r="57" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A57">
         <v>54</v>
       </c>
@@ -6498,7 +6495,7 @@
         <v>update lab set lab = 'Institute of Public Health', country = '' where lab_id = 54</v>
       </c>
     </row>
-    <row r="58" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A58">
         <v>55</v>
       </c>
@@ -6519,7 +6516,7 @@
         <v>update lab set lab = 'Higher Environmental Committee - Ministry of Health', country = '' where lab_id = 55</v>
       </c>
     </row>
-    <row r="59" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A59">
         <v>56</v>
       </c>
@@ -6540,7 +6537,7 @@
         <v>update lab set lab = '"Ruder Boskovic" Institute Centre for Marine Research', country = '' where lab_id = 56</v>
       </c>
     </row>
-    <row r="60" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A60">
         <v>57</v>
       </c>
@@ -6561,7 +6558,7 @@
         <v>update lab set lab = 'Ellauri 533', country = '' where lab_id = 57</v>
       </c>
     </row>
-    <row r="61" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A61">
         <v>58</v>
       </c>
@@ -6585,7 +6582,7 @@
         <v>update lab set lab = 'Chemical Engineer - S.O.H.M.A.', country = '' where lab_id = 58</v>
       </c>
     </row>
-    <row r="62" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A62">
         <v>59</v>
       </c>
@@ -6609,7 +6606,7 @@
         <v>update lab set lab = '"Ruder Boskovic" Institute - Centre for Marine Research Zagreb', country = '' where lab_id = 59</v>
       </c>
     </row>
-    <row r="63" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A63">
         <v>60</v>
       </c>
@@ -6630,7 +6627,7 @@
         <v>update lab set lab = 'Institute of Nuclear Research - Academia de Ciencias de Cuba', country = '' where lab_id = 60</v>
       </c>
     </row>
-    <row r="64" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A64">
         <v>61</v>
       </c>
@@ -6651,7 +6648,7 @@
         <v>update lab set lab = 'Catedra de Radioquimica - Facultad de Quimica', country = '' where lab_id = 61</v>
       </c>
     </row>
-    <row r="65" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="65" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A65">
         <v>62</v>
       </c>
@@ -6675,7 +6672,7 @@
         <v>update lab set lab = 'Centro de Proteccion e Hygiene de las Radiaciones', country = '' where lab_id = 62</v>
       </c>
     </row>
-    <row r="66" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="66" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A66">
         <v>63</v>
       </c>
@@ -6699,7 +6696,7 @@
         <v>update lab set lab = 'Ministry of Agriculture and Natural Resources', country = '' where lab_id = 63</v>
       </c>
     </row>
-    <row r="67" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="67" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A67">
         <v>64</v>
       </c>
@@ -6720,7 +6717,7 @@
         <v>update lab set lab = 'MEGA -  a.s.', country = '' where lab_id = 64</v>
       </c>
     </row>
-    <row r="68" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="68" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A68">
         <v>65</v>
       </c>
@@ -6741,7 +6738,7 @@
         <v>update lab set lab = 'Institute of Radioecology and Applied Nuclear Techniques', country = '' where lab_id = 65</v>
       </c>
     </row>
-    <row r="69" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="69" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A69">
         <v>66</v>
       </c>
@@ -6765,7 +6762,7 @@
         <v>update lab set lab = 'Laboratory of Spectrometry Centre of Radiation Hygiene', country = '' where lab_id = 66</v>
       </c>
     </row>
-    <row r="70" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="70" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A70">
         <v>67</v>
       </c>
@@ -6786,7 +6783,7 @@
         <v>update lab set lab = 'Research Institute of Preventive Medicine', country = '' where lab_id = 67</v>
       </c>
     </row>
-    <row r="71" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="71" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A71">
         <v>68</v>
       </c>
@@ -6807,7 +6804,7 @@
         <v>update lab set lab = 'Geological Survey', country = '' where lab_id = 68</v>
       </c>
     </row>
-    <row r="72" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="72" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A72">
         <v>69</v>
       </c>
@@ -6831,7 +6828,7 @@
         <v>update lab set lab = 'V U J E - Nuclear Power Plants', country = '' where lab_id = 69</v>
       </c>
     </row>
-    <row r="73" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="73" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A73">
         <v>70</v>
       </c>
@@ -6852,7 +6849,7 @@
         <v>update lab set lab = 'Harvard University - Harvard University Center for the Environment', country = '' where lab_id = 70</v>
       </c>
     </row>
-    <row r="74" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="74" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A74">
         <v>71</v>
       </c>
@@ -6876,7 +6873,7 @@
         <v>update lab set lab = 'Comision Ecuatoriana de Energia Atomica', country = '' where lab_id = 71</v>
       </c>
     </row>
-    <row r="75" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="75" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A75">
         <v>72</v>
       </c>
@@ -6900,7 +6897,7 @@
         <v>update lab set lab = 'Institute of Oceanography and Fisheries', country = '' where lab_id = 72</v>
       </c>
     </row>
-    <row r="76" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="76" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A76">
         <v>73</v>
       </c>
@@ -6924,7 +6921,7 @@
         <v>update lab set lab = 'Institute of Graduate Studies and Research', country = '' where lab_id = 73</v>
       </c>
     </row>
-    <row r="77" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="77" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A77">
         <v>74</v>
       </c>
@@ -6948,7 +6945,7 @@
         <v>update lab set lab = 'Nuclear Power Plants Authority', country = '' where lab_id = 74</v>
       </c>
     </row>
-    <row r="78" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="78" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A78">
         <v>75</v>
       </c>
@@ -6969,7 +6966,7 @@
         <v>update lab set lab = 'Institute of Biology of South Seas - Academy of Sciences of Ukraine', country = '' where lab_id = 75</v>
       </c>
     </row>
-    <row r="79" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A79">
         <v>76</v>
       </c>
@@ -6993,7 +6990,7 @@
         <v>update lab set lab = 'Environmental and Occupational Health Centre', country = '' where lab_id = 76</v>
       </c>
     </row>
-    <row r="80" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="80" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A80">
         <v>77</v>
       </c>
@@ -7020,7 +7017,7 @@
         <v>update lab set lab = 'Finnish Centre for Radiation and Nuclear Safety', country = '' where lab_id = 77</v>
       </c>
     </row>
-    <row r="81" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A81">
         <v>78</v>
       </c>
@@ -7044,7 +7041,7 @@
         <v>update lab set lab = 'Laboratoire de Radiochimie - Faculté des Sciences', country = '' where lab_id = 78</v>
       </c>
     </row>
-    <row r="82" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="82" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A82">
         <v>79</v>
       </c>
@@ -7065,7 +7062,7 @@
         <v>update lab set lab = 'Marine Hydrophysical Institute - Academy of Sciences of Ukraine', country = '' where lab_id = 79</v>
       </c>
     </row>
-    <row r="83" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="83" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A83">
         <v>80</v>
       </c>
@@ -7092,7 +7089,7 @@
         <v>update lab set lab = 'Commissariat à l'énergie atomique et aux énergies alternatives', country = '' where lab_id = 80</v>
       </c>
     </row>
-    <row r="84" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A84">
         <v>81</v>
       </c>
@@ -7119,7 +7116,7 @@
         <v>update lab set lab = 'Lawrence Livermore National Laboratory', country = '' where lab_id = 81</v>
       </c>
     </row>
-    <row r="85" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="85" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A85">
         <v>82</v>
       </c>
@@ -7143,7 +7140,7 @@
         <v>update lab set lab = 'COGEMA - Groupe Environnement', country = '' where lab_id = 82</v>
       </c>
     </row>
-    <row r="86" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="86" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A86">
         <v>83</v>
       </c>
@@ -7167,7 +7164,7 @@
         <v>update lab set lab = 'Commissariat à l'énergie atomique et aux énergies alternatives - Direction Centrale - SMSR', country = '' where lab_id = 83</v>
       </c>
     </row>
-    <row r="87" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="87" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A87">
         <v>84</v>
       </c>
@@ -7191,7 +7188,7 @@
         <v>update lab set lab = 'Centre de Recherches du Service de Santé des Armées', country = '' where lab_id = 84</v>
       </c>
     </row>
-    <row r="88" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="88" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A88">
         <v>85</v>
       </c>
@@ -7215,7 +7212,7 @@
         <v>update lab set lab = 'I.P.S.N. - DPEI/SERE (LMEI)', country = '' where lab_id = 85</v>
       </c>
     </row>
-    <row r="89" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="89" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A89">
         <v>86</v>
       </c>
@@ -7239,7 +7236,7 @@
         <v>update lab set lab = 'IFREMER - Centre de Toulon (CEA - S.M.T.)', country = '' where lab_id = 86</v>
       </c>
     </row>
-    <row r="90" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="90" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A90">
         <v>87</v>
       </c>
@@ -7263,7 +7260,7 @@
         <v>update lab set lab = 'Laboratoire de Radioécologie des Eaux Continentales', country = '' where lab_id = 87</v>
       </c>
     </row>
-    <row r="91" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="91" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A91">
         <v>88</v>
       </c>
@@ -7281,7 +7278,7 @@
         <v>update lab set lab = 'Institut de Protection et de Sûreté Nucléaire - DPEI', country = '' where lab_id = 88</v>
       </c>
     </row>
-    <row r="92" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="92" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A92">
         <v>89</v>
       </c>
@@ -7302,7 +7299,7 @@
         <v>update lab set lab = 'Marine Nationale Section de Surveillance Radiologique', country = '' where lab_id = 89</v>
       </c>
     </row>
-    <row r="93" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="93" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A93">
         <v>90</v>
       </c>
@@ -7320,7 +7317,7 @@
         <v>update lab set lab = 'Centre des Faibles Radioactivités - Laboratoire Mixte CNRS-CEA', country = '' where lab_id = 90</v>
       </c>
     </row>
-    <row r="94" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="94" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A94">
         <v>91</v>
       </c>
@@ -7344,7 +7341,7 @@
         <v>update lab set lab = 'Service de Sécurité Radiologique du port de Brest', country = '' where lab_id = 91</v>
       </c>
     </row>
-    <row r="95" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A95">
         <v>92</v>
       </c>
@@ -7365,7 +7362,7 @@
         <v>update lab set lab = 'Institut de Biogéochimie Marine - Ecole Normale Supérieure  (ENS)', country = '' where lab_id = 92</v>
       </c>
     </row>
-    <row r="96" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="96" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A96">
         <v>93</v>
       </c>
@@ -7389,7 +7386,7 @@
         <v>update lab set lab = 'Universidad Simon Bolivar - Laboratorio de Fisica Nuclear', country = '' where lab_id = 93</v>
       </c>
     </row>
-    <row r="97" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A97">
         <v>94</v>
       </c>
@@ -7413,7 +7410,7 @@
         <v>update lab set lab = 'Institut de Protection et de Sûreté Nucléaire - Lab. d'Etude et de Surveillance de l'Environnement', country = '' where lab_id = 94</v>
       </c>
     </row>
-    <row r="98" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="98" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A98">
         <v>95</v>
       </c>
@@ -7437,7 +7434,7 @@
         <v>update lab set lab = 'Kernforschungszentrum Karlsruhe Hauptabteilung Sicherheit', country = '' where lab_id = 95</v>
       </c>
     </row>
-    <row r="99" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="99" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A99">
         <v>96</v>
       </c>
@@ -7458,7 +7455,7 @@
         <v>update lab set lab = 'Institut für Wässer Boden und Lufthygiene des Bundesgesund.', country = '' where lab_id = 96</v>
       </c>
     </row>
-    <row r="100" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="100" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A100">
         <v>97</v>
       </c>
@@ -7482,7 +7479,7 @@
         <v>update lab set lab = 'Landesuntersuchungsamt für das Gesundheitswesen Nordbayern', country = '' where lab_id = 97</v>
       </c>
     </row>
-    <row r="101" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="101" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A101">
         <v>98</v>
       </c>
@@ -7503,7 +7500,7 @@
         <v>update lab set lab = 'Ingenieurgesellschaft IAF', country = '' where lab_id = 98</v>
       </c>
     </row>
-    <row r="102" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="102" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A102">
         <v>99</v>
       </c>
@@ -7524,7 +7521,7 @@
         <v>update lab set lab = 'Institut für Wabohu-Hygiene (Labor BI 2)', country = '' where lab_id = 99</v>
       </c>
     </row>
-    <row r="103" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="103" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A103">
         <v>100</v>
       </c>
@@ -7548,7 +7545,7 @@
         <v>update lab set lab = 'Laboratorio de Espectroscopia Atomica y Nuclear', country = '' where lab_id = 100</v>
       </c>
     </row>
-    <row r="104" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="104" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A104">
         <v>101</v>
       </c>
@@ -7572,7 +7569,7 @@
         <v>update lab set lab = 'Sektion Physik - WB Angewandte Physik', country = '' where lab_id = 101</v>
       </c>
     </row>
-    <row r="105" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="105" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A105">
         <v>102</v>
       </c>
@@ -7596,7 +7593,7 @@
         <v>update lab set lab = 'IVIC - Lab. de Mineralogia', country = '' where lab_id = 102</v>
       </c>
     </row>
-    <row r="106" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="106" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A106">
         <v>103</v>
       </c>
@@ -7620,7 +7617,7 @@
         <v>update lab set lab = 'Verein für Kernverfahrenstechnik und Analytik Rossendorf e.V.', country = '' where lab_id = 103</v>
       </c>
     </row>
-    <row r="107" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="107" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A107">
         <v>104</v>
       </c>
@@ -7644,7 +7641,7 @@
         <v>update lab set lab = 'GKSS - Forschungszentrum Geesthacht', country = '' where lab_id = 104</v>
       </c>
     </row>
-    <row r="108" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="108" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A108">
         <v>105</v>
       </c>
@@ -7671,7 +7668,7 @@
         <v>update lab set lab = 'Bundesforschungsanstalt für fisher.', country = '' where lab_id = 105</v>
       </c>
     </row>
-    <row r="109" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="109" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A109">
         <v>106</v>
       </c>
@@ -7695,7 +7692,7 @@
         <v>update lab set lab = 'Hessische', country = '' where lab_id = 106</v>
       </c>
     </row>
-    <row r="110" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="110" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A110">
         <v>107</v>
       </c>
@@ -7716,7 +7713,7 @@
         <v>update lab set lab = 'Strahlenbiologisches Institut der Universität München', country = '' where lab_id = 107</v>
       </c>
     </row>
-    <row r="111" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="111" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A111">
         <v>108</v>
       </c>
@@ -7737,7 +7734,7 @@
         <v>update lab set lab = 'Staatliches amt für Atomsicherheit und Strahlenschutz', country = '' where lab_id = 108</v>
       </c>
     </row>
-    <row r="112" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="112" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A112">
         <v>109</v>
       </c>
@@ -7761,7 +7758,7 @@
         <v>update lab set lab = 'Fachbereich Physikalische Chemie der Philipps - Universitaet', country = '' where lab_id = 109</v>
       </c>
     </row>
-    <row r="113" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A113">
         <v>110</v>
       </c>
@@ -7785,7 +7782,7 @@
         <v>update lab set lab = 'Federal Maritime and Hydrographic Agency', country = '' where lab_id = 110</v>
       </c>
     </row>
-    <row r="114" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="114" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A114">
         <v>111</v>
       </c>
@@ -7806,7 +7803,7 @@
         <v>update lab set lab = 'Zentralinstitut für Kernforschung Rossendorf', country = '' where lab_id = 111</v>
       </c>
     </row>
-    <row r="115" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="115" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A115">
         <v>112</v>
       </c>
@@ -7827,7 +7824,7 @@
         <v>update lab set lab = 'Nuclear Research Institute', country = '' where lab_id = 112</v>
       </c>
     </row>
-    <row r="116" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A116">
         <v>113</v>
       </c>
@@ -7845,7 +7842,7 @@
         <v>update lab set lab = 'Institute of Applied Physical Chem. - Nuclear Research Centre - Jülich', country = '' where lab_id = 113</v>
       </c>
     </row>
-    <row r="117" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A117">
         <v>114</v>
       </c>
@@ -7869,7 +7866,7 @@
         <v>update lab set lab = 'Akademie der Wissenschaften - Zentralinstitut für Kernforschung', country = '' where lab_id = 114</v>
       </c>
     </row>
-    <row r="118" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="118" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A118">
         <v>115</v>
       </c>
@@ -7890,7 +7887,7 @@
         <v>update lab set lab = 'Kernforschungszentrum Karlsruhe (BFE  BAU 325)', country = '' where lab_id = 115</v>
       </c>
     </row>
-    <row r="119" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="119" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A119">
         <v>116</v>
       </c>
@@ -7911,7 +7908,7 @@
         <v>update lab set lab = 'Vietnam National Atomic Energy Commission', country = '' where lab_id = 116</v>
       </c>
     </row>
-    <row r="120" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="120" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A120">
         <v>117</v>
       </c>
@@ -7932,7 +7929,7 @@
         <v>update lab set lab = 'Niedersaechsisches Landesamt für Wasser und Abfall', country = '' where lab_id = 117</v>
       </c>
     </row>
-    <row r="121" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A121">
         <v>118</v>
       </c>
@@ -7953,7 +7950,7 @@
         <v>update lab set lab = 'National Board of Nuclear Safety and Radiation Protection', country = '' where lab_id = 118</v>
       </c>
     </row>
-    <row r="122" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="122" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A122">
         <v>119</v>
       </c>
@@ -7974,7 +7971,7 @@
         <v>update lab set lab = 'Bergakademie Freiberg - Sektion Physik', country = '' where lab_id = 119</v>
       </c>
     </row>
-    <row r="123" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="123" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A123">
         <v>120</v>
       </c>
@@ -7998,7 +7995,7 @@
         <v>update lab set lab = 'Physikalisch-Technische Bundesanst.', country = '' where lab_id = 120</v>
       </c>
     </row>
-    <row r="124" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="124" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A124">
         <v>121</v>
       </c>
@@ -8019,7 +8016,7 @@
         <v>update lab set lab = 'Dept. of Physics/Reactor Technology - Ghana Atomic Energy Commission', country = '' where lab_id = 121</v>
       </c>
     </row>
-    <row r="125" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="125" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A125">
         <v>122</v>
       </c>
@@ -8043,7 +8040,7 @@
         <v>update lab set lab = 'NCSR "Demokritos" - Institute of Nuclear Technology', country = '' where lab_id = 122</v>
       </c>
     </row>
-    <row r="126" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="126" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A126">
         <v>123</v>
       </c>
@@ -8064,7 +8061,7 @@
         <v>update lab set lab = 'Royal Observatory - Hong Kong Government', country = '' where lab_id = 123</v>
       </c>
     </row>
-    <row r="127" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A127">
         <v>124</v>
       </c>
@@ -8085,7 +8082,7 @@
         <v>update lab set lab = 'National Research Institute for Radiobiology &amp; Radiohygiene', country = '' where lab_id = 124</v>
       </c>
     </row>
-    <row r="128" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A128">
         <v>125</v>
       </c>
@@ -8109,7 +8106,7 @@
         <v>update lab set lab = 'Radiological Sciences Institute - Division of Labs. &amp; Research', country = '' where lab_id = 125</v>
       </c>
     </row>
-    <row r="129" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="129" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A129">
         <v>126</v>
       </c>
@@ -8130,7 +8127,7 @@
         <v>update lab set lab = 'Department of Applied Chemistry - Technical University of Budapest', country = '' where lab_id = 126</v>
       </c>
     </row>
-    <row r="130" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="130" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A130">
         <v>127</v>
       </c>
@@ -8154,7 +8151,7 @@
         <v>update lab set lab = 'University of Utah - School of Medicine', country = '' where lab_id = 127</v>
       </c>
     </row>
-    <row r="131" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="131" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A131">
         <v>128</v>
       </c>
@@ -8175,7 +8172,7 @@
         <v>update lab set lab = 'Central Research Institute for Physics of the Hungarian Academy of Sciences-Health Physics Dept.', country = '' where lab_id = 128</v>
       </c>
     </row>
-    <row r="132" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="132" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A132">
         <v>129</v>
       </c>
@@ -8196,7 +8193,7 @@
         <v>update lab set lab = 'Environmental Studies Section - Health Physics Division', country = '' where lab_id = 129</v>
       </c>
     </row>
-    <row r="133" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="133" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A133">
         <v>130</v>
       </c>
@@ -8220,7 +8217,7 @@
         <v>update lab set lab = 'Research and Development Centre for Oceanology', country = '' where lab_id = 130</v>
       </c>
     </row>
-    <row r="134" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="134" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A134">
         <v>131</v>
       </c>
@@ -8244,7 +8241,7 @@
         <v>update lab set lab = 'Centre for the Application of Isotopes and Radiation', country = '' where lab_id = 131</v>
       </c>
     </row>
-    <row r="135" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="135" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A135">
         <v>132</v>
       </c>
@@ -8265,7 +8262,7 @@
         <v>update lab set lab = 'Radiation Protection Department - Atomic Energy Organization of Iran', country = '' where lab_id = 132</v>
       </c>
     </row>
-    <row r="136" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="136" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A136">
         <v>133</v>
       </c>
@@ -8289,7 +8286,7 @@
         <v>update lab set lab = 'Nuclear Research Centre - Department of Ecology', country = '' where lab_id = 133</v>
       </c>
     </row>
-    <row r="137" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="137" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A137">
         <v>134</v>
       </c>
@@ -8313,7 +8310,7 @@
         <v>update lab set lab = 'University of Pittsburg - Radiochemical Analytical Laboratory', country = '' where lab_id = 134</v>
       </c>
     </row>
-    <row r="138" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="138" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A138">
         <v>135</v>
       </c>
@@ -8337,7 +8334,7 @@
         <v>update lab set lab = 'Nuclear Energy Board', country = '' where lab_id = 135</v>
       </c>
     </row>
-    <row r="139" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="139" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A139">
         <v>136</v>
       </c>
@@ -8361,7 +8358,7 @@
         <v>update lab set lab = 'Physics Dept. - University College', country = '' where lab_id = 136</v>
       </c>
     </row>
-    <row r="140" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="140" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A140">
         <v>137</v>
       </c>
@@ -8382,7 +8379,7 @@
         <v>update lab set lab = 'E.N.E.A. - Centro Ricerche Nucl. della Trisaia', country = '' where lab_id = 137</v>
       </c>
     </row>
-    <row r="141" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="141" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A141">
         <v>138</v>
       </c>
@@ -8406,7 +8403,7 @@
         <v>update lab set lab = 'Laboratorio di Metrologia delle Radiazioni Ionizzanti', country = '' where lab_id = 138</v>
       </c>
     </row>
-    <row r="142" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="142" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A142">
         <v>139</v>
       </c>
@@ -8433,7 +8430,7 @@
         <v>update lab set lab = 'E.N.E.A. - Centro Ricerche Energia Ambiente', country = '' where lab_id = 139</v>
       </c>
     </row>
-    <row r="143" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="143" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A143">
         <v>140</v>
       </c>
@@ -8454,7 +8451,7 @@
         <v>update lab set lab = 'E.N.E.A. - C.R.E.  Brasimone', country = '' where lab_id = 140</v>
       </c>
     </row>
-    <row r="144" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="144" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A144">
         <v>141</v>
       </c>
@@ -8475,7 +8472,7 @@
         <v>update lab set lab = 'Istituto di Zoologia', country = '' where lab_id = 141</v>
       </c>
     </row>
-    <row r="145" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="145" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A145">
         <v>142</v>
       </c>
@@ -8496,7 +8493,7 @@
         <v>update lab set lab = 'Istituto di Ingegneria Nucleare Politecnico di Milano', country = '' where lab_id = 142</v>
       </c>
     </row>
-    <row r="146" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="146" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A146">
         <v>143</v>
       </c>
@@ -8517,7 +8514,7 @@
         <v>update lab set lab = 'University of Parma - Dipartimento di Biologia', country = '' where lab_id = 143</v>
       </c>
     </row>
-    <row r="147" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="147" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A147">
         <v>144</v>
       </c>
@@ -8538,7 +8535,7 @@
         <v>update lab set lab = 'Institute of Chemistry - University of Tsukuba', country = '' where lab_id = 144</v>
       </c>
     </row>
-    <row r="148" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="148" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A148">
         <v>145</v>
       </c>
@@ -8562,7 +8559,7 @@
         <v>update lab set lab = 'Power Reactor Nuclear Fuel - Development Corporation', country = '' where lab_id = 145</v>
       </c>
     </row>
-    <row r="149" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="149" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A149">
         <v>146</v>
       </c>
@@ -8586,7 +8583,7 @@
         <v>update lab set lab = 'Japan Atomic Energy Research Institute', country = '' where lab_id = 146</v>
       </c>
     </row>
-    <row r="150" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="150" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A150">
         <v>147</v>
       </c>
@@ -8610,7 +8607,7 @@
         <v>update lab set lab = 'Japan Chemical Analysis Centre', country = '' where lab_id = 147</v>
       </c>
     </row>
-    <row r="151" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="151" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A151">
         <v>148</v>
       </c>
@@ -8634,7 +8631,7 @@
         <v>update lab set lab = 'University of Tokyo - Ocean Research Institute', country = '' where lab_id = 148</v>
       </c>
     </row>
-    <row r="152" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="152" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A152">
         <v>149</v>
       </c>
@@ -8655,7 +8652,7 @@
         <v>update lab set lab = 'Kanazawa University - Faculty of Science', country = '' where lab_id = 149</v>
       </c>
     </row>
-    <row r="153" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="153" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A153">
         <v>150</v>
       </c>
@@ -8679,7 +8676,7 @@
         <v>update lab set lab = 'M.A.D. Group/HASRD - Oak Ridge National Laboratory', country = '' where lab_id = 150</v>
       </c>
     </row>
-    <row r="154" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="154" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A154">
         <v>151</v>
       </c>
@@ -8700,7 +8697,7 @@
         <v>update lab set lab = 'Hokkaido University - Faculty of Fisheries', country = '' where lab_id = 151</v>
       </c>
     </row>
-    <row r="155" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="155" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A155">
         <v>152</v>
       </c>
@@ -8724,7 +8721,7 @@
         <v>update lab set lab = 'Kanazawa University - Low Level Radioactivity Laboratory', country = '' where lab_id = 152</v>
       </c>
     </row>
-    <row r="156" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="156" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A156">
         <v>153</v>
       </c>
@@ -8745,7 +8742,7 @@
         <v>update lab set lab = 'Marine Biogeochemistry - Korea Ocean Research and Development Institute', country = '' where lab_id = 153</v>
       </c>
     </row>
-    <row r="157" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="157" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A157">
         <v>154</v>
       </c>
@@ -8769,7 +8766,7 @@
         <v>update lab set lab = '4th Division of Instruments - Korea Basic Science Centre', country = '' where lab_id = 154</v>
       </c>
     </row>
-    <row r="158" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="158" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A158">
         <v>155</v>
       </c>
@@ -8790,7 +8787,7 @@
         <v>update lab set lab = 'Kuwait Scientific Research Instit. - Central Analytical Laboratory', country = '' where lab_id = 155</v>
       </c>
     </row>
-    <row r="159" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="159" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A159">
         <v>156</v>
       </c>
@@ -8811,7 +8808,7 @@
         <v>update lab set lab = 'Ministry of Public Health - Environmental Protection Dept.', country = '' where lab_id = 156</v>
       </c>
     </row>
-    <row r="160" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="160" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A160">
         <v>157</v>
       </c>
@@ -8832,7 +8829,7 @@
         <v>update lab set lab = 'Conseil National de la Recherche Scientifique', country = '' where lab_id = 157</v>
       </c>
     </row>
-    <row r="161" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="161" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A161">
         <v>158</v>
       </c>
@@ -8853,7 +8850,7 @@
         <v>update lab set lab = 'Tajoura Research Centre', country = '' where lab_id = 158</v>
       </c>
     </row>
-    <row r="162" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="162" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A162">
         <v>159</v>
       </c>
@@ -8874,7 +8871,7 @@
         <v>update lab set lab = 'Nationwide Radiological Study', country = '' where lab_id = 159</v>
       </c>
     </row>
-    <row r="163" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="163" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A163">
         <v>160</v>
       </c>
@@ -8898,7 +8895,7 @@
         <v>update lab set lab = 'C.N.S.N.S. - Env. Radiation Surveillance Branch', country = '' where lab_id = 160</v>
       </c>
     </row>
-    <row r="164" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="164" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A164">
         <v>161</v>
       </c>
@@ -8925,7 +8922,7 @@
         <v>update lab set lab = 'Radiological &amp; Env. Sciences Lab. - Department of Energy', country = '' where lab_id = 161</v>
       </c>
     </row>
-    <row r="165" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="165" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A165">
         <v>162</v>
       </c>
@@ -8949,7 +8946,7 @@
         <v>update lab set lab = 'Instituto de Investig. Electricas - Interior Internado Palmira', country = '' where lab_id = 162</v>
       </c>
     </row>
-    <row r="166" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="166" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A166">
         <v>163</v>
       </c>
@@ -8973,7 +8970,7 @@
         <v>update lab set lab = 'Laboratorio de Dosimetria y Monitoreo Ambiental - CFE - GCN', country = '' where lab_id = 163</v>
       </c>
     </row>
-    <row r="167" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="167" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A167">
         <v>164</v>
       </c>
@@ -8994,7 +8991,7 @@
         <v>update lab set lab = 'Laboratoire de Physique Nucléaire - Faculté des Sciences', country = '' where lab_id = 164</v>
       </c>
     </row>
-    <row r="168" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="168" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A168">
         <v>165</v>
       </c>
@@ -9018,7 +9015,7 @@
         <v>update lab set lab = 'Institut National Agronomique et Vétérinaire Hassan II', country = '' where lab_id = 165</v>
       </c>
     </row>
-    <row r="169" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="169" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A169">
         <v>166</v>
       </c>
@@ -9036,7 +9033,7 @@
         <v>update lab set lab = 'Ecole Mohammadia d'Ingénieurs - Centre National de Génie Sanitaire', country = '' where lab_id = 166</v>
       </c>
     </row>
-    <row r="170" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="170" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A170">
         <v>167</v>
       </c>
@@ -9057,7 +9054,7 @@
         <v>update lab set lab = 'Netherlands Institute for Sea Research (N.I.O.Z.)', country = '' where lab_id = 167</v>
       </c>
     </row>
-    <row r="171" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="171" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A171">
         <v>168</v>
       </c>
@@ -9078,7 +9075,7 @@
         <v>update lab set lab = 'Nat. Air &amp; Radiat. Environmental Lab. - U.S. Environmental Protection Agency', country = '' where lab_id = 168</v>
       </c>
     </row>
-    <row r="172" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="172" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A172">
         <v>169</v>
       </c>
@@ -9099,7 +9096,7 @@
         <v>update lab set lab = 'RIVM - Laboratory for Radiation Research', country = '' where lab_id = 169</v>
       </c>
     </row>
-    <row r="173" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="173" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A173">
         <v>170</v>
       </c>
@@ -9123,7 +9120,7 @@
         <v>update lab set lab = 'Radiochemistry Dept. of the Radiation Research Laboratory', country = '' where lab_id = 170</v>
       </c>
     </row>
-    <row r="174" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="174" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A174">
         <v>171</v>
       </c>
@@ -9144,7 +9141,7 @@
         <v>update lab set lab = 'Food Inspection Service', country = '' where lab_id = 171</v>
       </c>
     </row>
-    <row r="175" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="175" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A175">
         <v>172</v>
       </c>
@@ -9165,7 +9162,7 @@
         <v>update lab set lab = 'Rijksinstituut voor Volksgesondheid en Milieu Hygiene', country = '' where lab_id = 172</v>
       </c>
     </row>
-    <row r="176" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="176" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A176">
         <v>173</v>
       </c>
@@ -9186,7 +9183,7 @@
         <v>update lab set lab = 'Interfaculty Reactor Institute', country = '' where lab_id = 173</v>
       </c>
     </row>
-    <row r="177" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="177" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A177">
         <v>174</v>
       </c>
@@ -9210,7 +9207,7 @@
         <v>update lab set lab = 'Instit. for Inland Water Management and Waste Water Treatment', country = '' where lab_id = 174</v>
       </c>
     </row>
-    <row r="178" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="178" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A178">
         <v>175</v>
       </c>
@@ -9234,7 +9231,7 @@
         <v>update lab set lab = 'Netherlands Energy Research Foundation ECN', country = '' where lab_id = 175</v>
       </c>
     </row>
-    <row r="179" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="179" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A179">
         <v>176</v>
       </c>
@@ -9255,7 +9252,7 @@
         <v>update lab set lab = 'RIKILT', country = '' where lab_id = 176</v>
       </c>
     </row>
-    <row r="180" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="180" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A180">
         <v>177</v>
       </c>
@@ -9273,7 +9270,7 @@
         <v>update lab set lab = 'Environmental Sciences Division - Oak Ridge National Laboratory', country = '' where lab_id = 177</v>
       </c>
     </row>
-    <row r="181" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="181" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A181">
         <v>178</v>
       </c>
@@ -9294,7 +9291,7 @@
         <v>update lab set lab = 'Institute of Nuclear Sciences', country = '' where lab_id = 178</v>
       </c>
     </row>
-    <row r="182" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="182" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A182">
         <v>179</v>
       </c>
@@ -9315,7 +9312,7 @@
         <v>update lab set lab = 'Centre for Energy Research and Training', country = '' where lab_id = 179</v>
       </c>
     </row>
-    <row r="183" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="183" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A183">
         <v>180</v>
       </c>
@@ -9336,7 +9333,7 @@
         <v>update lab set lab = 'Institute for Energy Technology Health and Safety Department', country = '' where lab_id = 180</v>
       </c>
     </row>
-    <row r="184" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="184" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A184">
         <v>181</v>
       </c>
@@ -9357,7 +9354,7 @@
         <v>update lab set lab = 'National Institute for Radiation Hygiene', country = '' where lab_id = 181</v>
       </c>
     </row>
-    <row r="185" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="185" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A185">
         <v>182</v>
       </c>
@@ -9378,7 +9375,7 @@
         <v>update lab set lab = 'PINSTECH', country = '' where lab_id = 182</v>
       </c>
     </row>
-    <row r="186" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="186" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A186">
         <v>183</v>
       </c>
@@ -9402,7 +9399,7 @@
         <v>update lab set lab = 'Instituto Peruano de Energia Nuclear', country = '' where lab_id = 183</v>
       </c>
     </row>
-    <row r="187" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="187" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A187">
         <v>184</v>
       </c>
@@ -9426,7 +9423,7 @@
         <v>update lab set lab = 'Philippine Nuclear Research Inst. - Health Physics Research', country = '' where lab_id = 184</v>
       </c>
     </row>
-    <row r="188" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="188" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A188">
         <v>185</v>
       </c>
@@ -9447,7 +9444,7 @@
         <v>update lab set lab = 'Radiological Services Section - Environmental Management Dept.', country = '' where lab_id = 185</v>
       </c>
     </row>
-    <row r="189" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="189" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A189">
         <v>186</v>
       </c>
@@ -9468,7 +9465,7 @@
         <v>update lab set lab = 'Nuclear Reactor Laboratory - Ohio State University', country = '' where lab_id = 186</v>
       </c>
     </row>
-    <row r="190" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="190" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A190">
         <v>187</v>
       </c>
@@ -9489,7 +9486,7 @@
         <v>update lab set lab = 'Institute of Oceanology - PAN', country = '' where lab_id = 187</v>
       </c>
     </row>
-    <row r="191" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="191" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A191">
         <v>188</v>
       </c>
@@ -9513,7 +9510,7 @@
         <v>update lab set lab = 'Central Laboratory for Radiological Protection', country = '' where lab_id = 188</v>
       </c>
     </row>
-    <row r="192" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="192" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A192">
         <v>189</v>
       </c>
@@ -9537,7 +9534,7 @@
         <v>update lab set lab = 'Department of Chemistry - Wyzsza Szkola Polniczo-Pedagocicna', country = '' where lab_id = 189</v>
       </c>
     </row>
-    <row r="193" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="193" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A193">
         <v>190</v>
       </c>
@@ -9555,7 +9552,7 @@
         <v>update lab set lab = 'University of Arkansas - Department of Chemistry', country = '' where lab_id = 190</v>
       </c>
     </row>
-    <row r="194" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="194" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A194">
         <v>191</v>
       </c>
@@ -9579,7 +9576,7 @@
         <v>update lab set lab = 'Institute of Meteorology and Water Management', country = '' where lab_id = 191</v>
       </c>
     </row>
-    <row r="195" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="195" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A195">
         <v>192</v>
       </c>
@@ -9603,7 +9600,7 @@
         <v>update lab set lab = 'Instytut Chemie Inorganicznej - Metallurgii Pierwiastkow Rzadkich', country = '' where lab_id = 192</v>
       </c>
     </row>
-    <row r="196" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="196" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A196">
         <v>193</v>
       </c>
@@ -9627,7 +9624,7 @@
         <v>update lab set lab = 'LNETI - Dept. de Protec. e Segur. Radiolog.', country = '' where lab_id = 193</v>
       </c>
     </row>
-    <row r="197" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="197" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A197">
         <v>194</v>
       </c>
@@ -9648,7 +9645,7 @@
         <v>update lab set lab = 'University of Southern California - Dept. of Geological Sciences', country = '' where lab_id = 194</v>
       </c>
     </row>
-    <row r="198" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="198" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A198">
         <v>195</v>
       </c>
@@ -9672,7 +9669,7 @@
         <v>update lab set lab = 'Romanian Marine Research Institute - Radiobiology Unit', country = '' where lab_id = 195</v>
       </c>
     </row>
-    <row r="199" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="199" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A199">
         <v>196</v>
       </c>
@@ -9690,7 +9687,7 @@
         <v>update lab set lab = 'Environmental Laboratory SPECTRA Ltd. (ul. Chopina 15)', country = '' where lab_id = 196</v>
       </c>
     </row>
-    <row r="200" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="200" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A200">
         <v>197</v>
       </c>
@@ -9711,7 +9708,7 @@
         <v>update lab set lab = 'Department of Radiology (339 MRB Building)', country = '' where lab_id = 197</v>
       </c>
     </row>
-    <row r="201" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="201" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A201">
         <v>198</v>
       </c>
@@ -9732,7 +9729,7 @@
         <v>update lab set lab = 'Laboratory for Air Pollution and Environmental Radioactivity', country = '' where lab_id = 198</v>
       </c>
     </row>
-    <row r="202" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="202" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A202">
         <v>199</v>
       </c>
@@ -9756,7 +9753,7 @@
         <v>update lab set lab = 'D345 - Lab. of Inorg. &amp; Nuclear Chem. - Wadsworth Center for Labs &amp; Research', country = '' where lab_id = 199</v>
       </c>
     </row>
-    <row r="203" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="203" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A203">
         <v>200</v>
       </c>
@@ -9777,7 +9774,7 @@
         <v>update lab set lab = 'Institute for Physics and Nuclear Engineering', country = '' where lab_id = 200</v>
       </c>
     </row>
-    <row r="204" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="204" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A204">
         <v>201</v>
       </c>
@@ -9801,7 +9798,7 @@
         <v>update lab set lab = 'Scientific Research. - Institute of Food Chemistry', country = '' where lab_id = 201</v>
       </c>
     </row>
-    <row r="205" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="205" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A205">
         <v>202</v>
       </c>
@@ -9825,7 +9822,7 @@
         <v>update lab set lab = 'Polytechnic Institute', country = '' where lab_id = 202</v>
       </c>
     </row>
-    <row r="206" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="206" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A206">
         <v>203</v>
       </c>
@@ -9852,7 +9849,7 @@
         <v>update lab set lab = 'E.M.L. - Department of Energy', country = '' where lab_id = 203</v>
       </c>
     </row>
-    <row r="207" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="207" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A207">
         <v>204</v>
       </c>
@@ -9873,7 +9870,7 @@
         <v>update lab set lab = 'Radiation Hygiene Laboratory - Inst. for Hygiene &amp; Public Health', country = '' where lab_id = 204</v>
       </c>
     </row>
-    <row r="208" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="208" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A208">
         <v>205</v>
       </c>
@@ -9903,7 +9900,7 @@
         <v>update lab set lab = 'Environmental Radioactivity Lab. - Inst. of Environmental Research and Engineering', country = '40(0)552695' where lab_id = 205</v>
       </c>
     </row>
-    <row r="209" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="209" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A209">
         <v>206</v>
       </c>
@@ -9924,7 +9921,7 @@
         <v>update lab set lab = 'Institute of Atomic Physics', country = '' where lab_id = 206</v>
       </c>
     </row>
-    <row r="210" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="210" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A210">
         <v>207</v>
       </c>
@@ -9945,7 +9942,7 @@
         <v>update lab set lab = 'Institute for Nucl. Power Reactors - Environmental Monitoring Laboratory', country = '' where lab_id = 207</v>
       </c>
     </row>
-    <row r="211" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="211" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A211">
         <v>208</v>
       </c>
@@ -9963,7 +9960,7 @@
         <v>update lab set lab = 'The Florida State University Department of Oceanography', country = '' where lab_id = 208</v>
       </c>
     </row>
-    <row r="212" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="212" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A212">
         <v>209</v>
       </c>
@@ -9984,7 +9981,7 @@
         <v>update lab set lab = 'National Radiological Protection Board', country = '' where lab_id = 209</v>
       </c>
     </row>
-    <row r="213" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="213" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A213">
         <v>210</v>
       </c>
@@ -10005,7 +10002,7 @@
         <v>update lab set lab = 'Director of VNIIGEOINFORSISTEM (for V.V. Millera)', country = '' where lab_id = 210</v>
       </c>
     </row>
-    <row r="214" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="214" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A214">
         <v>211</v>
       </c>
@@ -10026,7 +10023,7 @@
         <v>update lab set lab = 'V.G. Khlopin Radium Institute - Lab. of Environmental Radioactive Contamination Monitoring', country = '' where lab_id = 211</v>
       </c>
     </row>
-    <row r="215" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="215" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A215">
         <v>212</v>
       </c>
@@ -10047,7 +10044,7 @@
         <v>update lab set lab = 'Polytechnic Institute - Geological Faculty', country = '' where lab_id = 212</v>
       </c>
     </row>
-    <row r="216" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="216" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A216">
         <v>213</v>
       </c>
@@ -10068,7 +10065,7 @@
         <v>update lab set lab = 'Radiometry &amp; Radioecology Laboratory - Agriculture University', country = '' where lab_id = 213</v>
       </c>
     </row>
-    <row r="217" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="217" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A217">
         <v>214</v>
       </c>
@@ -10086,7 +10083,7 @@
         <v>update lab set lab = 'Research Institute - University of Petroleum &amp; Minerals', country = '' where lab_id = 214</v>
       </c>
     </row>
-    <row r="218" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="218" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A218">
         <v>215</v>
       </c>
@@ -10110,7 +10107,7 @@
         <v>update lab set lab = 'Institute of Occupational Health Radiological Protection', country = '' where lab_id = 215</v>
       </c>
     </row>
-    <row r="219" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="219" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A219">
         <v>216</v>
       </c>
@@ -10131,7 +10128,7 @@
         <v>update lab set lab = 'Zavod SRS za varstvo pri delu', country = '' where lab_id = 216</v>
       </c>
     </row>
-    <row r="220" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="220" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A220">
         <v>217</v>
       </c>
@@ -10155,7 +10152,7 @@
         <v>update lab set lab = 'Nuclear Institute "Jozef Stefan"', country = '' where lab_id = 217</v>
       </c>
     </row>
-    <row r="221" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="221" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A221">
         <v>218</v>
       </c>
@@ -10176,7 +10173,7 @@
         <v>update lab set lab = 'Importing Company IRIS', country = '' where lab_id = 218</v>
       </c>
     </row>
-    <row r="222" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="222" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A222">
         <v>219</v>
       </c>
@@ -10200,7 +10197,7 @@
         <v>update lab set lab = 'Environmental Studies Subdivision - Isotopes and Radiation Department', country = '' where lab_id = 219</v>
       </c>
     </row>
-    <row r="223" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="223" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A223">
         <v>220</v>
       </c>
@@ -10221,7 +10218,7 @@
         <v>update lab set lab = 'Council for Nuclear Safety', country = '' where lab_id = 220</v>
       </c>
     </row>
-    <row r="224" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="224" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A224">
         <v>221</v>
       </c>
@@ -10242,7 +10239,7 @@
         <v>update lab set lab = 'Koeberg Nuclear Power Station - Environmental Survey Laboratory', country = '' where lab_id = 221</v>
       </c>
     </row>
-    <row r="225" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="225" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A225">
         <v>222</v>
       </c>
@@ -10263,7 +10260,7 @@
         <v>update lab set lab = 'Cardiff City Analysts', country = '' where lab_id = 222</v>
       </c>
     </row>
-    <row r="226" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="226" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A226">
         <v>223</v>
       </c>
@@ -10284,7 +10281,7 @@
         <v>update lab set lab = 'Universidad de Sevilla - Facultad de Fisica', country = '' where lab_id = 223</v>
       </c>
     </row>
-    <row r="227" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="227" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A227">
         <v>224</v>
       </c>
@@ -10305,7 +10302,7 @@
         <v>update lab set lab = 'Nuclear Chemistry Division - Pakistan Institute of Nuclear Science and Technology', country = '' where lab_id = 224</v>
       </c>
     </row>
-    <row r="228" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="228" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A228">
         <v>225</v>
       </c>
@@ -10326,7 +10323,7 @@
         <v>update lab set lab = 'CIEMAT (I.M.A.) Ed.3', country = '' where lab_id = 225</v>
       </c>
     </row>
-    <row r="229" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="229" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A229">
         <v>226</v>
       </c>
@@ -10347,7 +10344,7 @@
         <v>update lab set lab = 'University of Extremadura - Facultad de Veterinaria', country = '' where lab_id = 226</v>
       </c>
     </row>
-    <row r="230" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="230" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A230">
         <v>227</v>
       </c>
@@ -10368,7 +10365,7 @@
         <v>update lab set lab = 'Instituto de Fisica Corpuscular', country = '' where lab_id = 227</v>
       </c>
     </row>
-    <row r="231" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="231" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A231">
         <v>228</v>
       </c>
@@ -10392,7 +10389,7 @@
         <v>update lab set lab = 'Instituto de Tecnicas Energeticas - Univers. Politecnicas Barcelona', country = '' where lab_id = 228</v>
       </c>
     </row>
-    <row r="232" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="232" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A232">
         <v>229</v>
       </c>
@@ -10416,7 +10413,7 @@
         <v>update lab set lab = 'Jefe Seccion Analisis y Medidas', country = '' where lab_id = 229</v>
       </c>
     </row>
-    <row r="233" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="233" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A233">
         <v>230</v>
       </c>
@@ -10437,7 +10434,7 @@
         <v>update lab set lab = 'Servei de Fisica de les Radiacions - Universitat Autonoma de Barcelona', country = '' where lab_id = 230</v>
       </c>
     </row>
-    <row r="234" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="234" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A234">
         <v>231</v>
       </c>
@@ -10458,7 +10455,7 @@
         <v>update lab set lab = 'Geotecnia y Cimientos S.A. - Poligono Industrial de Coslada', country = '' where lab_id = 231</v>
       </c>
     </row>
-    <row r="235" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="235" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A235">
         <v>232</v>
       </c>
@@ -10479,7 +10476,7 @@
         <v>update lab set lab = 'AEA - Environment and Energy Business', country = '' where lab_id = 232</v>
       </c>
     </row>
-    <row r="236" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="236" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A236">
         <v>233</v>
       </c>
@@ -10500,7 +10497,7 @@
         <v>update lab set lab = 'Institute of Oceanographic Sciences', country = '' where lab_id = 233</v>
       </c>
     </row>
-    <row r="237" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="237" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A237">
         <v>234</v>
       </c>
@@ -10524,7 +10521,7 @@
         <v>update lab set lab = 'Environmental Study Unit - National Aquatic Resources Agency', country = '' where lab_id = 234</v>
       </c>
     </row>
-    <row r="238" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="238" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A238">
         <v>235</v>
       </c>
@@ -10545,7 +10542,7 @@
         <v>update lab set lab = 'Council for Conservation of Environment', country = '' where lab_id = 235</v>
       </c>
     </row>
-    <row r="239" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="239" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A239">
         <v>236</v>
       </c>
@@ -10566,7 +10563,7 @@
         <v>update lab set lab = 'Ministry of Environment (Sultanate of Oman)', country = '' where lab_id = 236</v>
       </c>
     </row>
-    <row r="240" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="240" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A240">
         <v>237</v>
       </c>
@@ -10584,7 +10581,7 @@
         <v>update lab set lab = 'Lund University - Department of Radiation Physics', country = '' where lab_id = 237</v>
       </c>
     </row>
-    <row r="241" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="241" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A241">
         <v>238</v>
       </c>
@@ -10614,7 +10611,7 @@
         <v>update lab set lab = 'The Swedish University of Agricultural Sciences', country = '46 018 671000' where lab_id = 238</v>
       </c>
     </row>
-    <row r="242" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="242" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A242">
         <v>239</v>
       </c>
@@ -10638,7 +10635,7 @@
         <v>update lab set lab = 'Swedish Environment Protection Agency', country = '46 08 7991061' where lab_id = 239</v>
       </c>
     </row>
-    <row r="243" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="243" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A243">
         <v>240</v>
       </c>
@@ -10656,7 +10653,7 @@
         <v>update lab set lab = 'Studsvik Nuclear AB', country = '' where lab_id = 240</v>
       </c>
     </row>
-    <row r="244" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="244" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A244">
         <v>241</v>
       </c>
@@ -10683,7 +10680,7 @@
         <v>update lab set lab = 'The Swedish Radiation Protection Authority/National Institute of Radiation Protection', country = '' where lab_id = 241</v>
       </c>
     </row>
-    <row r="245" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="245" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A245">
         <v>242</v>
       </c>
@@ -10704,7 +10701,7 @@
         <v>update lab set lab = 'N.R.P.B. - Scottish Centre', country = '' where lab_id = 242</v>
       </c>
     </row>
-    <row r="246" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="246" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A246">
         <v>243</v>
       </c>
@@ -10728,7 +10725,7 @@
         <v>update lab set lab = 'National Defence Research Institute', country = '' where lab_id = 243</v>
       </c>
     </row>
-    <row r="247" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="247" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A247">
         <v>244</v>
       </c>
@@ -10749,7 +10746,7 @@
         <v>update lab set lab = 'Institut F.A. Forel - Université de Genève', country = '' where lab_id = 244</v>
       </c>
     </row>
-    <row r="248" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="248" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A248">
         <v>245</v>
       </c>
@@ -10770,7 +10767,7 @@
         <v>update lab set lab = 'Paul Scherrer Institute', country = '' where lab_id = 245</v>
       </c>
     </row>
-    <row r="249" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="249" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A249">
         <v>246</v>
       </c>
@@ -10791,7 +10788,7 @@
         <v>update lab set lab = 'Université de Neuchatel - Groupe Prosper', country = '' where lab_id = 246</v>
       </c>
     </row>
-    <row r="250" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="250" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A250">
         <v>247</v>
       </c>
@@ -10812,7 +10809,7 @@
         <v>update lab set lab = 'EAWAG - Abwasserreinigung u. Gewässerschutz', country = '' where lab_id = 247</v>
       </c>
     </row>
-    <row r="251" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="251" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A251">
         <v>248</v>
       </c>
@@ -10836,7 +10833,7 @@
         <v>update lab set lab = 'Federal Office of Public Health - Radiation Surveillance Section', country = '' where lab_id = 248</v>
       </c>
     </row>
-    <row r="252" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="252" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A252">
         <v>249</v>
       </c>
@@ -10860,7 +10857,7 @@
         <v>update lab set lab = 'Radiation Measurement Division (Bangkok)', country = '' where lab_id = 249</v>
       </c>
     </row>
-    <row r="253" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="253" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A253">
         <v>250</v>
       </c>
@@ -10881,7 +10878,7 @@
         <v>update lab set lab = 'Napier Polytechnic of Edinburgh', country = '' where lab_id = 250</v>
       </c>
     </row>
-    <row r="254" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="254" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A254">
         <v>251</v>
       </c>
@@ -10905,7 +10902,7 @@
         <v>update lab set lab = 'Office of Atomic Energy for Peace - Env. Radiation Poll. Studies Sect.', country = '' where lab_id = 251</v>
       </c>
     </row>
-    <row r="255" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="255" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A255">
         <v>252</v>
       </c>
@@ -10926,7 +10923,7 @@
         <v>update lab set lab = 'Institut National Scientifique et Technique d'Océanographie et de Pêches', country = '' where lab_id = 252</v>
       </c>
     </row>
-    <row r="256" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="256" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A256">
         <v>253</v>
       </c>
@@ -10947,7 +10944,7 @@
         <v>update lab set lab = 'Karadeniz Teknik Universitesi - Radiobiology Laboratory', country = '' where lab_id = 253</v>
       </c>
     </row>
-    <row r="257" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="257" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A257">
         <v>254</v>
       </c>
@@ -10968,7 +10965,7 @@
         <v>update lab set lab = 'Cekmece Nuclear Research and Training Centre', country = '' where lab_id = 254</v>
       </c>
     </row>
-    <row r="258" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="258" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A258">
         <v>255</v>
       </c>
@@ -10989,7 +10986,7 @@
         <v>update lab set lab = 'Technical University of Istanbul - Institute for Nuclear Energy', country = '' where lab_id = 255</v>
       </c>
     </row>
-    <row r="259" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="259" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A259">
         <v>256</v>
       </c>
@@ -11013,7 +11010,7 @@
         <v>update lab set lab = 'EGE University - Faculty of Science - Hydrology Laboratory', country = '' where lab_id = 256</v>
       </c>
     </row>
-    <row r="260" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="260" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A260">
         <v>257</v>
       </c>
@@ -11034,7 +11031,7 @@
         <v>update lab set lab = 'MAFF (Staplake Mount)', country = '' where lab_id = 257</v>
       </c>
     </row>
-    <row r="261" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="261" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A261">
         <v>258</v>
       </c>
@@ -11058,7 +11055,7 @@
         <v>update lab set lab = 'N.R.P.B. (Northern Centre)', country = '' where lab_id = 258</v>
       </c>
     </row>
-    <row r="262" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="262" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A262">
         <v>259</v>
       </c>
@@ -11076,7 +11073,7 @@
         <v>update lab set lab = 'Department of Environmental Science - University of Lancaster', country = '' where lab_id = 259</v>
       </c>
     </row>
-    <row r="263" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="263" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A263">
         <v>260</v>
       </c>
@@ -11097,7 +11094,7 @@
         <v>update lab set lab = 'UKA.E.A. Technology - Dounreay Nuclear Power', country = '' where lab_id = 260</v>
       </c>
     </row>
-    <row r="264" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="264" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A264">
         <v>261</v>
       </c>
@@ -11121,7 +11118,7 @@
         <v>update lab set lab = 'British Nuclear Fuels plc - Chemical &amp; Metallurgical Services', country = '' where lab_id = 261</v>
       </c>
     </row>
-    <row r="265" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="265" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A265">
         <v>262</v>
       </c>
@@ -11142,7 +11139,7 @@
         <v>update lab set lab = 'Central Electricity Generating Bd. - Scientific and Technical Branch', country = '' where lab_id = 262</v>
       </c>
     </row>
-    <row r="266" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="266" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A266">
         <v>263</v>
       </c>
@@ -11163,7 +11160,7 @@
         <v>update lab set lab = 'Department of Regional Chemist - Public Analyst and Agric. Analyst', country = '' where lab_id = 263</v>
       </c>
     </row>
-    <row r="267" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="267" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A267">
         <v>264</v>
       </c>
@@ -11184,7 +11181,7 @@
         <v>update lab set lab = 'Regional Analyst's Lab.', country = '' where lab_id = 264</v>
       </c>
     </row>
-    <row r="268" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="268" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A268">
         <v>265</v>
       </c>
@@ -11208,7 +11205,7 @@
         <v>update lab set lab = 'MAFF (Directorate of Fisheries Research)', country = '' where lab_id = 265</v>
       </c>
     </row>
-    <row r="269" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="269" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A269">
         <v>266</v>
       </c>
@@ -11229,7 +11226,7 @@
         <v>update lab set lab = 'Somerset County Council - County Laboratory', country = '' where lab_id = 266</v>
       </c>
     </row>
-    <row r="270" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="270" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A270">
         <v>267</v>
       </c>
@@ -11253,7 +11250,7 @@
         <v>update lab set lab = 'Division of Radiation Science and Acoustics', country = '' where lab_id = 267</v>
       </c>
     </row>
-    <row r="271" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="271" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A271">
         <v>268</v>
       </c>
@@ -11277,7 +11274,7 @@
         <v>update lab set lab = 'Institute of Environmental and Biological Sciences', country = '' where lab_id = 268</v>
       </c>
     </row>
-    <row r="272" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="272" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A272">
         <v>269</v>
       </c>
@@ -11301,7 +11298,7 @@
         <v>update lab set lab = 'Humberside County', country = '' where lab_id = 269</v>
       </c>
     </row>
-    <row r="273" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="273" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A273">
         <v>270</v>
       </c>
@@ -11319,7 +11316,7 @@
         <v>update lab set lab = 'Institute of Terrestrial Ecology - Merlewood Research Station', country = '' where lab_id = 270</v>
       </c>
     </row>
-    <row r="274" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="274" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A274">
         <v>271</v>
       </c>
@@ -11337,7 +11334,7 @@
         <v>update lab set lab = 'Chemistry Department - University of Glasgow', country = '' where lab_id = 271</v>
       </c>
     </row>
-    <row r="275" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="275" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A275">
         <v>272</v>
       </c>
@@ -11361,7 +11358,7 @@
         <v>update lab set lab = 'Lab. de Tecnicas Analit. Nucleares - Depart. de Radioanalysis y Tecnicas Nucleares', country = '' where lab_id = 272</v>
       </c>
     </row>
-    <row r="276" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="276" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A276">
         <v>273</v>
       </c>
@@ -11379,7 +11376,7 @@
         <v>update lab set lab = 'Bundesamt für Seeschiffahrt und Hydrographie', country = '' where lab_id = 273</v>
       </c>
     </row>
-    <row r="277" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="277" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A277">
         <v>274</v>
       </c>
@@ -11400,7 +11397,7 @@
         <v>update lab set lab = 'Kiev State University - Inter-Branch Institute of Personal Retraining', country = '' where lab_id = 274</v>
       </c>
     </row>
-    <row r="278" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="278" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A278">
         <v>275</v>
       </c>
@@ -11424,7 +11421,7 @@
         <v>update lab set lab = 'All-Union Scientific Centre of Radiation Medicine', country = '' where lab_id = 275</v>
       </c>
     </row>
-    <row r="279" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="279" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A279">
         <v>276</v>
       </c>
@@ -11448,7 +11445,7 @@
         <v>update lab set lab = 'Scottish Universities Research and Nuclear Centre', country = '' where lab_id = 276</v>
       </c>
     </row>
-    <row r="280" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="280" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A280">
         <v>277</v>
       </c>
@@ -11466,7 +11463,7 @@
         <v>update lab set lab = 'Russian Federation (X + 1)', country = '' where lab_id = 277</v>
       </c>
     </row>
-    <row r="281" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="281" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A281">
         <v>278</v>
       </c>
@@ -11484,7 +11481,7 @@
         <v>update lab set lab = 'Ministry of Agriculture, Fisheries and Food', country = '' where lab_id = 278</v>
       </c>
     </row>
-    <row r="282" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="282" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A282">
         <v>279</v>
       </c>
@@ -11505,7 +11502,7 @@
         <v>update lab set lab = 'Technological Institute of Mazatlán', country = '' where lab_id = 279</v>
       </c>
     </row>
-    <row r="283" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="283" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A283">
         <v>280</v>
       </c>
@@ -11526,7 +11523,7 @@
         <v>update lab set lab = 'Ehime Prefectural Institute of Public Health and Environmental Science', country = '' where lab_id = 280</v>
       </c>
     </row>
-    <row r="284" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="284" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A284">
         <v>281</v>
       </c>
@@ -11544,7 +11541,7 @@
         <v>update lab set lab = 'Norwegian Polar Institute', country = '' where lab_id = 281</v>
       </c>
     </row>
-    <row r="285" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="285" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A285">
         <v>282</v>
       </c>
@@ -11571,7 +11568,7 @@
         <v>update lab set lab = 'Woods Hole Oceanographic Institution', country = '' where lab_id = 282</v>
       </c>
     </row>
-    <row r="286" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="286" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A286">
         <v>283</v>
       </c>
@@ -11595,7 +11592,7 @@
         <v>update lab set lab = 'Indústrias Nucleares do Brasil', country = '' where lab_id = 283</v>
       </c>
     </row>
-    <row r="287" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="287" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A287">
         <v>284</v>
       </c>
@@ -11616,7 +11613,7 @@
         <v>update lab set lab = 'Bangladesh Atomic Energy Commission - Radioactivity Testing and Monitoring Laboratory', country = '' where lab_id = 284</v>
       </c>
     </row>
-    <row r="288" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="288" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A288">
         <v>285</v>
       </c>
@@ -11637,7 +11634,7 @@
         <v>update lab set lab = 'Scott Christian College - Department of Zoology and Research Centre', country = '' where lab_id = 285</v>
       </c>
     </row>
-    <row r="289" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="289" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A289">
         <v>286</v>
       </c>
@@ -11658,7 +11655,7 @@
         <v>update lab set lab = 'JSS University - Center for Water and Health', country = '' where lab_id = 286</v>
       </c>
     </row>
-    <row r="290" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="290" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A290">
         <v>287</v>
       </c>
@@ -11679,7 +11676,7 @@
         <v>update lab set lab = 'Sadakathullah Appa College - Department of Advanced Zoology and Biotechnology', country = '' where lab_id = 287</v>
       </c>
     </row>
-    <row r="291" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="291" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A291">
         <v>288</v>
       </c>
@@ -11700,7 +11697,7 @@
         <v>update lab set lab = 'ICAR-Central Institute of Fisheries Education', country = '' where lab_id = 288</v>
       </c>
     </row>
-    <row r="292" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="292" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A292">
         <v>289</v>
       </c>
@@ -11718,7 +11715,7 @@
         <v>update lab set lab = 'Yarmouk University - Faculty of Science', country = '' where lab_id = 289</v>
       </c>
     </row>
-    <row r="293" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="293" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A293">
         <v>290</v>
       </c>
@@ -11739,7 +11736,7 @@
         <v>update lab set lab = 'Universiti Teknologi MARA - Faculty of Applied Sciences', country = '' where lab_id = 290</v>
       </c>
     </row>
-    <row r="294" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="294" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A294">
         <v>291</v>
       </c>
@@ -11760,7 +11757,7 @@
         <v>update lab set lab = 'University of New York - Institute of Environmental Medicine', country = '' where lab_id = 291</v>
       </c>
     </row>
-    <row r="295" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="295" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A295">
         <v>292</v>
       </c>
@@ -11781,7 +11778,7 @@
         <v>update lab set lab = 'Sunway University - School of Healthcare and Medical Sciences', country = '' where lab_id = 292</v>
       </c>
     </row>
-    <row r="296" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="296" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A296">
         <v>293</v>
       </c>
@@ -11802,7 +11799,7 @@
         <v>update lab set lab = 'Kyushu University - Radioisotope Center', country = '' where lab_id = 293</v>
       </c>
     </row>
-    <row r="297" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="297" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A297">
         <v>294</v>
       </c>
@@ -11820,7 +11817,7 @@
         <v>update lab set lab = 'Korea Research Institute of Standards and Science', country = '' where lab_id = 294</v>
       </c>
     </row>
-    <row r="298" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="298" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A298">
         <v>295</v>
       </c>
@@ -11838,7 +11835,7 @@
         <v>update lab set lab = 'Tsinghua University - Department of Engineering Physics', country = '' where lab_id = 295</v>
       </c>
     </row>
-    <row r="299" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="299" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A299">
         <v>296</v>
       </c>
@@ -11859,7 +11856,7 @@
         <v>update lab set lab = 'Toho University - Department of Biomolecular Science', country = '' where lab_id = 296</v>
       </c>
     </row>
-    <row r="300" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="300" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A300">
         <v>297</v>
       </c>
@@ -11880,7 +11877,7 @@
         <v>update lab set lab = 'Stanford University - Hopkins Marine Station', country = '' where lab_id = 297</v>
       </c>
     </row>
-    <row r="301" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="301" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A301">
         <v>298</v>
       </c>
@@ -11898,7 +11895,7 @@
         <v>update lab set lab = 'National Institute for Radiological Protection', country = '' where lab_id = 298</v>
       </c>
     </row>
-    <row r="302" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="302" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A302">
         <v>299</v>
       </c>
@@ -11919,7 +11916,7 @@
         <v>update lab set lab = 'Stony Brook University - School of Marine and Atmospheric Sciences', country = '' where lab_id = 299</v>
       </c>
     </row>
-    <row r="303" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="303" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A303">
         <v>300</v>
       </c>
@@ -11940,7 +11937,7 @@
         <v>update lab set lab = 'Kirklareli University - Department of Physics', country = '' where lab_id = 300</v>
       </c>
     </row>
-    <row r="304" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="304" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A304">
         <v>301</v>
       </c>
@@ -11961,7 +11958,7 @@
         <v>update lab set lab = 'Radiation and Nuclear Safety Authority', country = '' where lab_id = 301</v>
       </c>
     </row>
-    <row r="305" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="305" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A305">
         <v>302</v>
       </c>
@@ -11982,7 +11979,7 @@
         <v>update lab set lab = 'Universidad de Sevilla - Centro de Investigación, Tecnología e Innovación', country = '' where lab_id = 302</v>
       </c>
     </row>
-    <row r="306" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="306" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A306">
         <v>303</v>
       </c>
@@ -12003,7 +12000,7 @@
         <v>update lab set lab = 'Universitat Rovira i Virgili - School of Medicine', country = '' where lab_id = 303</v>
       </c>
     </row>
-    <row r="307" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="307" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A307">
         <v>304</v>
       </c>
@@ -12024,7 +12021,7 @@
         <v>update lab set lab = 'Institute for Nuclear Research and Nuclear Energy - Radiochemistry and Radioecology Department', country = '' where lab_id = 304</v>
       </c>
     </row>
-    <row r="308" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="308" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A308">
         <v>305</v>
       </c>
@@ -12045,7 +12042,7 @@
         <v>update lab set lab = 'Technology Development Department', country = '' where lab_id = 305</v>
       </c>
     </row>
-    <row r="309" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="309" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A309">
         <v>306</v>
       </c>
@@ -12066,7 +12063,7 @@
         <v>update lab set lab = ' Ibn Tofail University - Department of Physics', country = '' where lab_id = 306</v>
       </c>
     </row>
-    <row r="310" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="310" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A310">
         <v>307</v>
       </c>
@@ -12084,7 +12081,7 @@
         <v>update lab set lab = 'Akdeniz University - Department of Aquaculture, Faculty of Fisheries', country = '' where lab_id = 307</v>
       </c>
     </row>
-    <row r="311" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="311" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A311">
         <v>308</v>
       </c>
@@ -12102,7 +12099,7 @@
         <v>update lab set lab = 'University of Malaya - Department of Physics', country = '' where lab_id = 308</v>
       </c>
     </row>
-    <row r="312" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="312" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A312">
         <v>309</v>
       </c>
@@ -12120,7 +12117,7 @@
         <v>update lab set lab = 'Morsli Abdallah University - Department of Natural Sciences and Life', country = '' where lab_id = 309</v>
       </c>
     </row>
-    <row r="313" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="313" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A313">
         <v>310</v>
       </c>
@@ -12141,7 +12138,7 @@
         <v>update lab set lab = 'Marine Biological Research Institute of Japan Co., LTD', country = '' where lab_id = 310</v>
       </c>
     </row>
-    <row r="314" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="314" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A314">
         <v>311</v>
       </c>
@@ -12165,7 +12162,7 @@
         <v>update lab set lab = 'University of California - Division of Environmental Studies', country = '' where lab_id = 311</v>
       </c>
     </row>
-    <row r="315" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="315" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A315">
         <v>312</v>
       </c>
@@ -12186,7 +12183,7 @@
         <v>update lab set lab = 'Tokyo University of Marine Science and Technology', country = '' where lab_id = 312</v>
       </c>
     </row>
-    <row r="316" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="316" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A316">
         <v>313</v>
       </c>
@@ -12204,7 +12201,7 @@
         <v>update lab set lab = 'Deutsch Hydrographisches Inst', country = '' where lab_id = 313</v>
       </c>
     </row>
-    <row r="317" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="317" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A317">
         <v>317</v>
       </c>
@@ -12222,7 +12219,7 @@
         <v>update lab set lab = 'University of Miami (C-14 lab)', country = '' where lab_id = 317</v>
       </c>
     </row>
-    <row r="318" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="318" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A318">
         <v>318</v>
       </c>
@@ -12240,7 +12237,7 @@
         <v>update lab set lab = 'University of Washington (C-14 lab)', country = '' where lab_id = 318</v>
       </c>
     </row>
-    <row r="319" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="319" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A319">
         <v>319</v>
       </c>
@@ -12258,7 +12255,7 @@
         <v>update lab set lab = 'SPA Typhoon', country = '' where lab_id = 319</v>
       </c>
     </row>
-    <row r="320" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="320" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A320">
         <v>320</v>
       </c>
@@ -12276,7 +12273,7 @@
         <v>update lab set lab = 'Radiation Protection Authority', country = '' where lab_id = 320</v>
       </c>
     </row>
-    <row r="321" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="321" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A321">
         <v>321</v>
       </c>
@@ -12306,7 +12303,7 @@
         <v>update lab set lab = 'Estonian Meteorological and Hydrological Institute', country = '' where lab_id = 321</v>
       </c>
     </row>
-    <row r="322" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="322" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A322">
         <v>322</v>
       </c>
@@ -12345,7 +12342,7 @@
         <v>update lab set lab = 'Estonian Radiation Protection Centre', country = '372 660 33' where lab_id = 322</v>
       </c>
     </row>
-    <row r="323" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="323" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A323">
         <v>323</v>
       </c>
@@ -12363,7 +12360,7 @@
         <v>update lab set lab = 'Joint Research Center', country = '' where lab_id = 323</v>
       </c>
     </row>
-    <row r="324" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="324" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A324">
         <v>324</v>
       </c>
@@ -12381,7 +12378,7 @@
         <v>update lab set lab = 'Lithuanian Environmental Protection Agency', country = '' where lab_id = 324</v>
       </c>
     </row>
-    <row r="325" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="325" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A325">
         <v>325</v>
       </c>
@@ -12402,7 +12399,7 @@
         <v>update lab set lab = 'Latvian Environment Agency', country = '' where lab_id = 325</v>
       </c>
     </row>
-    <row r="326" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="326" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A326">
         <v>326</v>
       </c>
@@ -12420,7 +12417,7 @@
         <v>update lab set lab = 'Environmental Data Center of Latvia', country = '' where lab_id = 326</v>
       </c>
     </row>
-    <row r="327" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="327" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A327">
         <v>327</v>
       </c>
@@ -12438,7 +12435,7 @@
         <v>update lab set lab = 'Lielriga Regional Environmental Board', country = '' where lab_id = 327</v>
       </c>
     </row>
-    <row r="328" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="328" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A328">
         <v>328</v>
       </c>
@@ -12468,7 +12465,7 @@
         <v>update lab set lab = 'Scientific Institute of public health', country = '32.2.642.56.62' where lab_id = 328</v>
       </c>
     </row>
-    <row r="329" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="329" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A329">
         <v>329</v>
       </c>
@@ -12498,7 +12495,7 @@
         <v>update lab set lab = 'Risø National Laboratory - The Radiation Research Department', country = '45 4677 5340' where lab_id = 329</v>
       </c>
     </row>
-    <row r="330" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="330" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A330">
         <v>330</v>
       </c>
@@ -12534,7 +12531,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire', country = '33130154949' where lab_id = 330</v>
       </c>
     </row>
-    <row r="331" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="331" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A331">
         <v>331</v>
       </c>
@@ -12558,7 +12555,7 @@
         <v>update lab set lab = 'Laboratoire des Etalons et des Intercomparaisons', country = '' where lab_id = 331</v>
       </c>
     </row>
-    <row r="332" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="332" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A332">
         <v>332</v>
       </c>
@@ -12591,7 +12588,7 @@
         <v>update lab set lab = 'Federal Maritime and Hydrographic Agency', country = '494031903300' where lab_id = 332</v>
       </c>
     </row>
-    <row r="333" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="333" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A333">
         <v>333</v>
       </c>
@@ -12621,7 +12618,7 @@
         <v>update lab set lab = 'Radiological Protection Institute of Ireland', country = '' where lab_id = 333</v>
       </c>
     </row>
-    <row r="334" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="334" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A334">
         <v>334</v>
       </c>
@@ -12651,7 +12648,7 @@
         <v>update lab set lab = 'University College Dublin Department of Experimental Physics', country = '' where lab_id = 334</v>
       </c>
     </row>
-    <row r="335" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="335" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A335">
         <v>335</v>
       </c>
@@ -12690,7 +12687,7 @@
         <v>update lab set lab = 'Norwegian Radiation Protection Authority (NRPA)', country = '4767162535' where lab_id = 335</v>
       </c>
     </row>
-    <row r="336" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="336" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A336">
         <v>336</v>
       </c>
@@ -12717,7 +12714,7 @@
         <v>update lab set lab = 'Instituto Tecnológico e Nuclear', country = '351 21 9946317' where lab_id = 336</v>
       </c>
     </row>
-    <row r="337" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="337" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A337">
         <v>337</v>
       </c>
@@ -12753,7 +12750,7 @@
         <v>update lab set lab = 'Coordinadora del Programa Científico Técnico', country = '34 913357217' where lab_id = 337</v>
       </c>
     </row>
-    <row r="338" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="338" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A338">
         <v>338</v>
       </c>
@@ -12780,7 +12777,7 @@
         <v>update lab set lab = 'Swedish Radiation Protection Authority', country = '' where lab_id = 338</v>
       </c>
     </row>
-    <row r="339" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="339" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A339">
         <v>339</v>
       </c>
@@ -12813,7 +12810,7 @@
         <v>update lab set lab = 'Cefas Lowestoft Laboratory', country = '01502 524477' where lab_id = 339</v>
       </c>
     </row>
-    <row r="340" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="340" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A340">
         <v>340</v>
       </c>
@@ -12846,7 +12843,7 @@
         <v>update lab set lab = 'SVERIGE'S  STRÅL SÄKERHETS MYNDIGHETEN', country = '+46 8 799 40 00' where lab_id = 340</v>
       </c>
     </row>
-    <row r="341" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="341" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A341">
         <v>341</v>
       </c>
@@ -12879,7 +12876,7 @@
         <v>update lab set lab = 'BUNDESFORSCHUNGANSTALT FÜR FISCHEREI', country = '(0 40) 38 9050' where lab_id = 341</v>
       </c>
     </row>
-    <row r="342" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="342" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A342">
         <v>342</v>
       </c>
@@ -12915,7 +12912,7 @@
         <v>update lab set lab = 'JOHAN HEINRICH VON THÜNEN-INSTITUTE', country = '+49531-5961003' where lab_id = 342</v>
       </c>
     </row>
-    <row r="343" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="343" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A343">
         <v>343</v>
       </c>
@@ -12942,7 +12939,7 @@
         <v>update lab set lab = 'Meteorological Research Institute', country = '' where lab_id = 343</v>
       </c>
     </row>
-    <row r="344" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="344" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A344">
         <v>344</v>
       </c>
@@ -12969,7 +12966,7 @@
         <v>update lab set lab = 'Research Institute for Global Change', country = '' where lab_id = 344</v>
       </c>
     </row>
-    <row r="345" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="345" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A345">
         <v>345</v>
       </c>
@@ -12999,7 +12996,7 @@
         <v>update lab set lab = 'Laboratory of Ion Beam Physics (LIP), ETZ Zürich, Switzerland', country = '' where lab_id = 345</v>
       </c>
     </row>
-    <row r="346" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="346" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A346">
         <v>346</v>
       </c>
@@ -13026,7 +13023,7 @@
         <v>update lab set lab = 'Marine Ecology Research Institute', country = '' where lab_id = 346</v>
       </c>
     </row>
-    <row r="347" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="347" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A347">
         <v>347</v>
       </c>
@@ -13053,7 +13050,7 @@
         <v>update lab set lab = 'Fisheries Research Agency - Research Center for Fisheries Oceanography and Marine Ecosystem', country = '' where lab_id = 347</v>
       </c>
     </row>
-    <row r="348" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="348" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A348">
         <v>348</v>
       </c>
@@ -13080,7 +13077,7 @@
         <v>update lab set lab = 'Institute of Biogeosciences', country = '' where lab_id = 348</v>
       </c>
     </row>
-    <row r="349" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="349" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A349">
         <v>349</v>
       </c>
@@ -13104,7 +13101,7 @@
         <v>update lab set lab = 'Japan Atomic Energy Agency', country = '' where lab_id = 349</v>
       </c>
     </row>
-    <row r="350" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="350" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A350">
         <v>350</v>
       </c>
@@ -13140,7 +13137,7 @@
         <v>update lab set lab = 'Radiation Safety Department, Environmental Board', country = '+372 664 4900' where lab_id = 350</v>
       </c>
     </row>
-    <row r="351" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="351" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A351">
         <v>351</v>
       </c>
@@ -13155,7 +13152,7 @@
         <v>update lab set lab = 'DTU Nutech', country = '' where lab_id = 351</v>
       </c>
     </row>
-    <row r="352" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="352" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A352">
         <v>352</v>
       </c>
@@ -13170,7 +13167,7 @@
         <v>update lab set lab = 'EA-Environment Agency', country = '' where lab_id = 352</v>
       </c>
     </row>
-    <row r="353" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="353" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A353">
         <v>353</v>
       </c>
@@ -13185,7 +13182,7 @@
         <v>update lab set lab = 'Environmental Protection Agency', country = '' where lab_id = 353</v>
       </c>
     </row>
-    <row r="354" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="354" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A354">
         <v>354</v>
       </c>
@@ -13200,7 +13197,7 @@
         <v>update lab set lab = 'FSA-Food Standards Agency', country = '' where lab_id = 354</v>
       </c>
     </row>
-    <row r="355" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="355" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A355">
         <v>355</v>
       </c>
@@ -13215,7 +13212,7 @@
         <v>update lab set lab = 'Icelandic Radiation Safety Authority', country = '' where lab_id = 355</v>
       </c>
     </row>
-    <row r="356" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="356" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A356">
         <v>356</v>
       </c>
@@ -13233,7 +13230,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LERFA', country = '' where lab_id = 356</v>
       </c>
     </row>
-    <row r="357" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="357" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A357">
         <v>357</v>
       </c>
@@ -13251,7 +13248,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LRC', country = '' where lab_id = 357</v>
       </c>
     </row>
-    <row r="358" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="358" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A358">
         <v>358</v>
       </c>
@@ -13269,7 +13266,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LRC/LMRE', country = '' where lab_id = 358</v>
       </c>
     </row>
-    <row r="359" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="359" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A359">
         <v>359</v>
       </c>
@@ -13287,7 +13284,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LRC/LS3E', country = '' where lab_id = 359</v>
       </c>
     </row>
-    <row r="360" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="360" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A360">
         <v>360</v>
       </c>
@@ -13305,7 +13302,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LRC/LSE', country = '' where lab_id = 360</v>
       </c>
     </row>
-    <row r="361" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="361" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A361">
         <v>361</v>
       </c>
@@ -13323,7 +13320,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LS3E', country = '' where lab_id = 361</v>
       </c>
     </row>
-    <row r="362" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="362" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A362">
         <v>362</v>
       </c>
@@ -13341,7 +13338,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LSE', country = '' where lab_id = 362</v>
       </c>
     </row>
-    <row r="363" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="363" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A363">
         <v>363</v>
       </c>
@@ -13359,7 +13356,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LVRE', country = '' where lab_id = 363</v>
       </c>
     </row>
-    <row r="364" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="364" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A364">
         <v>364</v>
       </c>
@@ -13377,7 +13374,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : OPRI', country = '' where lab_id = 364</v>
       </c>
     </row>
-    <row r="365" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="365" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A365">
         <v>365</v>
       </c>
@@ -13395,7 +13392,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : OPRI-LVRE', country = '' where lab_id = 365</v>
       </c>
     </row>
-    <row r="366" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="366" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A366">
         <v>366</v>
       </c>
@@ -13410,7 +13407,7 @@
         <v>update lab set lab = 'Institute for Energy Technology', country = '' where lab_id = 366</v>
       </c>
     </row>
-    <row r="367" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="367" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A367">
         <v>367</v>
       </c>
@@ -13425,7 +13422,7 @@
         <v>update lab set lab = 'Institute for Energy Technology / Norwegian Radiation Protection Authority', country = '' where lab_id = 367</v>
       </c>
     </row>
-    <row r="368" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="368" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A368">
         <v>368</v>
       </c>
@@ -13449,7 +13446,7 @@
         <v>update lab set lab = 'Institute of Marine Research', country = '' where lab_id = 368</v>
       </c>
     </row>
-    <row r="369" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="369" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A369">
         <v>369</v>
       </c>
@@ -13464,7 +13461,7 @@
         <v>update lab set lab = 'Institute of Marine Research / Norwegian Radiation Protection Authority', country = '' where lab_id = 369</v>
       </c>
     </row>
-    <row r="370" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="370" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A370">
         <v>370</v>
       </c>
@@ -13479,7 +13476,7 @@
         <v>update lab set lab = 'Johann Heinrich von Thünen Institute (vTI)', country = '' where lab_id = 370</v>
       </c>
     </row>
-    <row r="371" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="371" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A371">
         <v>371</v>
       </c>
@@ -13494,7 +13491,7 @@
         <v>update lab set lab = 'NIEA-Northern Ireland Environment Agency', country = '' where lab_id = 371</v>
       </c>
     </row>
-    <row r="372" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="372" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A372">
         <v>372</v>
       </c>
@@ -13512,7 +13509,7 @@
         <v>update lab set lab = 'Norwegian Radiation Protection Authority', country = '' where lab_id = 372</v>
       </c>
     </row>
-    <row r="373" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="373" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A373">
         <v>373</v>
       </c>
@@ -13527,7 +13524,7 @@
         <v>update lab set lab = 'Nuclear Energy Research Centre', country = '' where lab_id = 373</v>
       </c>
     </row>
-    <row r="374" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="374" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A374">
         <v>374</v>
       </c>
@@ -13542,7 +13539,7 @@
         <v>update lab set lab = 'Nuclear Safety Council', country = '' where lab_id = 374</v>
       </c>
     </row>
-    <row r="375" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="375" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A375">
         <v>376</v>
       </c>
@@ -13557,7 +13554,7 @@
         <v>update lab set lab = 'Rijkswaterstaat Centre for Water Management', country = '' where lab_id = 376</v>
       </c>
     </row>
-    <row r="376" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="376" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A376">
         <v>377</v>
       </c>
@@ -13572,7 +13569,7 @@
         <v>update lab set lab = 'Rijkswaterstaat Laboratory CIV', country = '' where lab_id = 377</v>
       </c>
     </row>
-    <row r="377" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="377" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A377">
         <v>378</v>
       </c>
@@ -13587,7 +13584,7 @@
         <v>update lab set lab = 'Scientific Institute of Public Health', country = '' where lab_id = 378</v>
       </c>
     </row>
-    <row r="378" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="378" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A378">
         <v>379</v>
       </c>
@@ -13602,7 +13599,7 @@
         <v>update lab set lab = 'SCK•CEN', country = '' where lab_id = 379</v>
       </c>
     </row>
-    <row r="379" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="379" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A379">
         <v>380</v>
       </c>
@@ -13617,7 +13614,7 @@
         <v>update lab set lab = 'SEPA-Scottish Environment Protection Agency', country = '' where lab_id = 380</v>
       </c>
     </row>
-    <row r="380" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="380" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A380">
         <v>381</v>
       </c>
@@ -13632,7 +13629,7 @@
         <v>update lab set lab = 'Swedish Radiation Safety Authority', country = '' where lab_id = 381</v>
       </c>
     </row>
-    <row r="381" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="381" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A381">
         <v>382</v>
       </c>
@@ -13647,7 +13644,7 @@
         <v>update lab set lab = 'The Norwegian Food Control Authority', country = '' where lab_id = 382</v>
       </c>
     </row>
-    <row r="382" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="382" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A382">
         <v>383</v>
       </c>
@@ -13662,7 +13659,7 @@
         <v>update lab set lab = 'BEIS (formerly DECC)', country = '' where lab_id = 383</v>
       </c>
     </row>
-    <row r="383" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="383" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A383">
         <v>384</v>
       </c>
@@ -13677,7 +13674,7 @@
         <v>update lab set lab = 'Corystes 14/2004', country = '' where lab_id = 384</v>
       </c>
     </row>
-    <row r="384" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="384" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A384">
         <v>385</v>
       </c>
@@ -13692,7 +13689,7 @@
         <v>update lab set lab = 'Defra-Department for Environment,  Food and Rural Affairs', country = '' where lab_id = 385</v>
       </c>
     </row>
-    <row r="385" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="385" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A385">
         <v>386</v>
       </c>
@@ -13707,7 +13704,7 @@
         <v>update lab set lab = 'Endeavour 10/2004', country = '' where lab_id = 386</v>
       </c>
     </row>
-    <row r="386" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="386" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A386">
         <v>387</v>
       </c>
@@ -13722,7 +13719,7 @@
         <v>update lab set lab = 'Federal Maritime and Hydrographic Agency, Hamburg', country = '' where lab_id = 387</v>
       </c>
     </row>
-    <row r="387" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="387" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A387">
         <v>388</v>
       </c>
@@ -13740,7 +13737,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LRC/LS3E, LTE', country = '' where lab_id = 388</v>
       </c>
     </row>
-    <row r="388" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="388" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A388">
         <v>389</v>
       </c>
@@ -13758,7 +13755,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LRC/LS3E/LMN', country = '' where lab_id = 389</v>
       </c>
     </row>
-    <row r="389" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="389" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A389">
         <v>390</v>
       </c>
@@ -13776,7 +13773,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LRC/LS3E/RSMASS', country = '' where lab_id = 390</v>
       </c>
     </row>
-    <row r="390" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="390" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A390">
         <v>391</v>
       </c>
@@ -13794,7 +13791,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LRC/LSE/LMN', country = '' where lab_id = 391</v>
       </c>
     </row>
-    <row r="391" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="391" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A391">
         <v>392</v>
       </c>
@@ -13812,7 +13809,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LRC/LTE, LMN', country = '' where lab_id = 392</v>
       </c>
     </row>
-    <row r="392" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="392" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A392">
         <v>393</v>
       </c>
@@ -13830,7 +13827,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LS3E/Marine Nationale', country = '' where lab_id = 393</v>
       </c>
     </row>
-    <row r="393" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="393" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A393">
         <v>394</v>
       </c>
@@ -13848,7 +13845,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LS3E/RSMASS', country = '' where lab_id = 394</v>
       </c>
     </row>
-    <row r="394" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="394" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A394">
         <v>395</v>
       </c>
@@ -13866,7 +13863,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LSE/Marine Nationale', country = '' where lab_id = 395</v>
       </c>
     </row>
-    <row r="395" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="395" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A395">
         <v>396</v>
       </c>
@@ -13884,7 +13881,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LVRE/MN', country = '' where lab_id = 396</v>
       </c>
     </row>
-    <row r="396" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="396" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A396">
         <v>397</v>
       </c>
@@ -13902,7 +13899,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LVRE/RSMASS', country = '' where lab_id = 397</v>
       </c>
     </row>
-    <row r="397" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="397" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A397">
         <v>398</v>
       </c>
@@ -13920,7 +13917,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : OPRI-LVRE/MN', country = '' where lab_id = 398</v>
       </c>
     </row>
-    <row r="398" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="398" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A398">
         <v>399</v>
       </c>
@@ -13938,7 +13935,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : OPRI/DDASS', country = '' where lab_id = 399</v>
       </c>
     </row>
-    <row r="399" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="399" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A399">
         <v>400</v>
       </c>
@@ -13956,7 +13953,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : OPRI/MN', country = '' where lab_id = 400</v>
       </c>
     </row>
-    <row r="400" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="400" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A400">
         <v>401</v>
       </c>
@@ -13974,7 +13971,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire - LS3E/STEME (ALOKA)', country = '' where lab_id = 401</v>
       </c>
     </row>
-    <row r="401" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="401" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A401">
         <v>402</v>
       </c>
@@ -13992,7 +13989,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire - LSE/STEME (ALOKA)', country = '' where lab_id = 402</v>
       </c>
     </row>
-    <row r="402" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="402" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A402">
         <v>403</v>
       </c>
@@ -14016,7 +14013,7 @@
         <v>update lab set lab = 'The Central Research Institute of Electric Power Industry', country = '' where lab_id = 403</v>
       </c>
     </row>
-    <row r="403" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="403" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A403">
         <v>404</v>
       </c>
@@ -14037,7 +14034,7 @@
         <v>update lab set lab = 'Polish Academy of Sciences - Institute of Nuclear Physics', country = '' where lab_id = 404</v>
       </c>
     </row>
-    <row r="404" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="404" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A404">
         <v>405</v>
       </c>
@@ -14055,7 +14052,7 @@
         <v>update lab set lab = 'University of Miami', country = '' where lab_id = 405</v>
       </c>
     </row>
-    <row r="405" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="405" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A405">
         <v>406</v>
       </c>
@@ -14073,7 +14070,7 @@
         <v>update lab set lab = 'University of Washington', country = '' where lab_id = 406</v>
       </c>
     </row>
-    <row r="406" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="406" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A406">
         <v>407</v>
       </c>
@@ -14097,7 +14094,7 @@
         <v>update lab set lab = 'Scripps Institution of Oceanography', country = '' where lab_id = 407</v>
       </c>
     </row>
-    <row r="407" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="407" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A407">
         <v>408</v>
       </c>
@@ -14115,7 +14112,7 @@
         <v>update lab set lab = 'University of Southern California', country = '' where lab_id = 408</v>
       </c>
     </row>
-    <row r="408" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="408" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A408">
         <v>409</v>
       </c>
@@ -14139,7 +14136,7 @@
         <v>update lab set lab = 'Yale University', country = '' where lab_id = 409</v>
       </c>
     </row>
-    <row r="409" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="409" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A409">
         <v>410</v>
       </c>
@@ -14160,7 +14157,7 @@
         <v>update lab set lab = 'Radiation Protection Bureau, Health Canada', country = '' where lab_id = 410</v>
       </c>
     </row>
-    <row r="410" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="410" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A410">
         <v>411</v>
       </c>
@@ -14184,7 +14181,7 @@
         <v>update lab set lab = 'Fisheries and Oceans Canada', country = '' where lab_id = 411</v>
       </c>
     </row>
-    <row r="411" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="411" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A411">
         <v>412</v>
       </c>
@@ -14205,7 +14202,7 @@
         <v>update lab set lab = 'Orano (former Areva) NC La Hague', country = '' where lab_id = 412</v>
       </c>
     </row>
-    <row r="412" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="412" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A412">
         <v>413</v>
       </c>
@@ -14229,7 +14226,7 @@
         <v>update lab set lab = 'Association pour le Contrôle de la Radioactivité dans l'Ouest', country = '' where lab_id = 413</v>
       </c>
     </row>
-    <row r="413" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="413" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A413">
         <v>414</v>
       </c>
@@ -14253,7 +14250,7 @@
         <v>update lab set lab = 'Base navale - Laboratoire de Surveillance Radiologique (LSR) - Brest', country = '' where lab_id = 414</v>
       </c>
     </row>
-    <row r="414" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="414" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A414">
         <v>415</v>
       </c>
@@ -14277,7 +14274,7 @@
         <v>update lab set lab = 'Base navale - Laboratoire de Surveillance Radiologique (LSR) - Cherbourg', country = '' where lab_id = 415</v>
       </c>
     </row>
-    <row r="415" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="415" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A415">
         <v>416</v>
       </c>
@@ -14301,7 +14298,7 @@
         <v>update lab set lab = 'Base navale - Service de Protection Radiologique - Ile longue', country = '' where lab_id = 416</v>
       </c>
     </row>
-    <row r="416" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="416" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A416">
         <v>417</v>
       </c>
@@ -14325,7 +14322,7 @@
         <v>update lab set lab = 'Commission Locale d'Information (CLI) de Gravelines', country = '' where lab_id = 417</v>
       </c>
     </row>
-    <row r="417" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="417" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A417">
         <v>418</v>
       </c>
@@ -14349,7 +14346,7 @@
         <v>update lab set lab = 'Orano (former Areva) Malvési', country = '' where lab_id = 418</v>
       </c>
     </row>
-    <row r="418" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="418" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A418">
         <v>419</v>
       </c>
@@ -14373,7 +14370,7 @@
         <v>update lab set lab = 'EDF - Centre Nucléaire de Production d'Électricite de Flamanville', country = '' where lab_id = 419</v>
       </c>
     </row>
-    <row r="419" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="419" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A419">
         <v>420</v>
       </c>
@@ -14400,7 +14397,7 @@
         <v>update lab set lab = 'EDF - Centre Nucléaire de Production d'Électricite de Paluel', country = '' where lab_id = 420</v>
       </c>
     </row>
-    <row r="420" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="420" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A420">
         <v>421</v>
       </c>
@@ -14424,7 +14421,7 @@
         <v>update lab set lab = 'EDF - Centre Nucléaire de Production d'Électricite de Penly', country = '' where lab_id = 421</v>
       </c>
     </row>
-    <row r="421" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="421" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A421">
         <v>422</v>
       </c>
@@ -14442,7 +14439,7 @@
         <v>update lab set lab = 'EDF - Centre Nucléaire de Production d'Électricite de Blayais', country = '' where lab_id = 422</v>
       </c>
     </row>
-    <row r="422" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="422" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A422">
         <v>423</v>
       </c>
@@ -14460,7 +14457,7 @@
         <v>update lab set lab = 'EDF - Centre Nucléaire de Production d'Électricite de Gravelines', country = '' where lab_id = 423</v>
       </c>
     </row>
-    <row r="423" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="423" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A423">
         <v>424</v>
       </c>
@@ -14481,7 +14478,7 @@
         <v>update lab set lab = 'FBFC International', country = '' where lab_id = 424</v>
       </c>
     </row>
-    <row r="424" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="424" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A424">
         <v>425</v>
       </c>
@@ -14502,7 +14499,7 @@
         <v>update lab set lab = 'Orano (former Areva) Tricastin Réseau de Surveillance de l'Environnement (RSE)', country = '' where lab_id = 425</v>
       </c>
     </row>
-    <row r="425" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="425" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A425">
         <v>426</v>
       </c>
@@ -14526,7 +14523,7 @@
         <v>update lab set lab = 'Commission Locale d'Information Nucléaire (CLIN) du Blayais', country = '+33 5 56 99 51 20' where lab_id = 426</v>
       </c>
     </row>
-    <row r="426" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="426" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A426">
         <v>427</v>
       </c>
@@ -14547,7 +14544,7 @@
         <v>update lab set lab = 'Institut Laue-Langevin', country = '' where lab_id = 427</v>
       </c>
     </row>
-    <row r="427" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="427" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A427">
         <v>428</v>
       </c>
@@ -14568,7 +14565,7 @@
         <v>update lab set lab = 'LABEO Manche', country = '' where lab_id = 428</v>
       </c>
     </row>
-    <row r="428" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="428" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A428">
         <v>429</v>
       </c>
@@ -14592,7 +14589,7 @@
         <v>update lab set lab = 'Autorité de Sûreté Nucléaire (ASN)', country = '' where lab_id = 429</v>
       </c>
     </row>
-    <row r="429" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="429" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A429">
         <v>430</v>
       </c>
@@ -14619,7 +14616,7 @@
         <v>update lab set lab = 'Commissariat à l'énergie atomique et aux énergies alternatives - Paris-Saclay', country = '+33 1 69 08 60 00' where lab_id = 430</v>
       </c>
     </row>
-    <row r="430" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="430" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A430">
         <v>431</v>
       </c>
@@ -14643,7 +14640,7 @@
         <v>update lab set lab = 'National Oceanic and Atmospheric Administration (NOAA)', country = '' where lab_id = 431</v>
       </c>
     </row>
-    <row r="431" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="431" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A431">
         <v>432</v>
       </c>
@@ -14667,7 +14664,7 @@
         <v>update lab set lab = 'Qatar University', country = '' where lab_id = 432</v>
       </c>
     </row>
-    <row r="432" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="432" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A432">
         <v>433</v>
       </c>
@@ -14688,7 +14685,7 @@
         <v>update lab set lab = 'University of Hawaii', country = '' where lab_id = 433</v>
       </c>
     </row>
-    <row r="433" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="433" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A433">
         <v>434</v>
       </c>
@@ -14709,7 +14706,7 @@
         <v>update lab set lab = 'University College Cork', country = '' where lab_id = 434</v>
       </c>
     </row>
-    <row r="434" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="434" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A434">
         <v>435</v>
       </c>
@@ -14730,7 +14727,7 @@
         <v>update lab set lab = 'Rutgers University', country = '' where lab_id = 435</v>
       </c>
     </row>
-    <row r="435" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="435" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A435">
         <v>436</v>
       </c>
@@ -14754,7 +14751,7 @@
         <v>update lab set lab = 'Ispettorato Nazionale per la Sicurezza Nucleare e la Radioprotezione', country = '' where lab_id = 436</v>
       </c>
     </row>
-    <row r="436" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="436" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A436">
         <v>437</v>
       </c>
@@ -14775,7 +14772,7 @@
         <v>update lab set lab = 'University of Canterbury', country = '' where lab_id = 437</v>
       </c>
     </row>
-    <row r="437" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="437" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A437">
         <v>438</v>
       </c>
@@ -14796,7 +14793,7 @@
         <v>update lab set lab = 'Thünen Institute of Fisheries Ecology', country = '' where lab_id = 438</v>
       </c>
     </row>
-    <row r="438" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="438" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A438">
         <v>439</v>
       </c>
@@ -14817,7 +14814,7 @@
         <v>update lab set lab = 'C. Abdul Hakeem College', country = '' where lab_id = 439</v>
       </c>
     </row>
-    <row r="439" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="439" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A439">
         <v>440</v>
       </c>
@@ -14841,7 +14838,7 @@
         <v>update lab set lab = 'U.S. Department of Energy', country = '' where lab_id = 440</v>
       </c>
     </row>
-    <row r="440" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="440" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A440">
         <v>441</v>
       </c>
@@ -14862,7 +14859,7 @@
         <v>update lab set lab = 'Seoul National University', country = '' where lab_id = 441</v>
       </c>
     </row>
-    <row r="441" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="441" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A441">
         <v>442</v>
       </c>
@@ -14883,7 +14880,7 @@
         <v>update lab set lab = 'Los Alamos National Laboratory', country = '' where lab_id = 442</v>
       </c>
     </row>
-    <row r="442" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="442" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A442">
         <v>443</v>
       </c>
@@ -14904,7 +14901,7 @@
         <v>update lab set lab = 'University of Melbourne', country = '' where lab_id = 443</v>
       </c>
     </row>
-    <row r="443" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="443" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A443">
         <v>444</v>
       </c>
@@ -14925,7 +14922,7 @@
         <v>update lab set lab = 'Brookhaven National Laboratory', country = '' where lab_id = 444</v>
       </c>
     </row>
-    <row r="444" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="444" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A444">
         <v>445</v>
       </c>
@@ -14946,7 +14943,7 @@
         <v>update lab set lab = 'Hokkaido Pharmaceutical Association Public Health Examination Center', country = '' where lab_id = 445</v>
       </c>
     </row>
-    <row r="445" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="445" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A445">
         <v>446</v>
       </c>
@@ -14970,7 +14967,7 @@
         <v>update lab set lab = 'University of Cape Town', country = '' where lab_id = 446</v>
       </c>
     </row>
-    <row r="446" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="446" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A446">
         <v>447</v>
       </c>
@@ -14994,7 +14991,7 @@
         <v>update lab set lab = 'Leibniz Center for Tropical Marine Ecology', country = '' where lab_id = 447</v>
       </c>
     </row>
-    <row r="447" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="447" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A447">
         <v>448</v>
       </c>
@@ -15018,7 +15015,7 @@
         <v>update lab set lab = 'Universidade Federal Fluminense', country = '' where lab_id = 448</v>
       </c>
     </row>
-    <row r="448" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="448" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A448">
         <v>449</v>
       </c>
@@ -15042,7 +15039,7 @@
         <v>update lab set lab = 'University of California', country = '' where lab_id = 449</v>
       </c>
     </row>
-    <row r="449" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="449" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A449">
         <v>450</v>
       </c>
@@ -15063,7 +15060,7 @@
         <v>update lab set lab = 'Istanbul University', country = '' where lab_id = 450</v>
       </c>
     </row>
-    <row r="450" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="450" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A450">
         <v>451</v>
       </c>
@@ -15087,7 +15084,7 @@
         <v>update lab set lab = 'Bhabha Atomic Research Center', country = '' where lab_id = 451</v>
       </c>
     </row>
-    <row r="451" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="451" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A451">
         <v>452</v>
       </c>
@@ -15108,7 +15105,7 @@
         <v>update lab set lab = 'King Saud University', country = '' where lab_id = 452</v>
       </c>
     </row>
-    <row r="452" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="452" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A452">
         <v>453</v>
       </c>
@@ -15132,7 +15129,7 @@
         <v>update lab set lab = 'National Institute of Radiological Sciences', country = '' where lab_id = 453</v>
       </c>
     </row>
-    <row r="453" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="453" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A453">
         <v>454</v>
       </c>
@@ -15153,7 +15150,7 @@
         <v>update lab set lab = 'Department of Chemistry and Biochemistry - University of Mississippi', country = '' where lab_id = 454</v>
       </c>
     </row>
-    <row r="454" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="454" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A454">
         <v>455</v>
       </c>
@@ -15177,7 +15174,7 @@
         <v>update lab set lab = 'Marine Science Department - University of Connecticut', country = '' where lab_id = 455</v>
       </c>
     </row>
-    <row r="455" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="455" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A455">
         <v>456</v>
       </c>
@@ -15201,7 +15198,7 @@
         <v>update lab set lab = 'Ege University - Institute of Nuclear Sciences', country = '' where lab_id = 456</v>
       </c>
     </row>
-    <row r="456" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="456" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A456">
         <v>457</v>
       </c>
@@ -15225,7 +15222,7 @@
         <v>update lab set lab = 'Aix-Marseille University - Mediterranean Institute of Oceanography', country = '' where lab_id = 457</v>
       </c>
     </row>
-    <row r="457" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="457" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A457">
         <v>458</v>
       </c>
@@ -15246,7 +15243,7 @@
         <v>update lab set lab = 'International Laboratory of Marine Radioactivity, Musée Océanographique', country = '' where lab_id = 458</v>
       </c>
     </row>
-    <row r="458" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="458" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A458">
         <v>459</v>
       </c>
@@ -15267,7 +15264,7 @@
         <v>update lab set lab = 'Department of Bio-Medical Physics - University of Aberdeen', country = '' where lab_id = 459</v>
       </c>
     </row>
-    <row r="459" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="459" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A459">
         <v>460</v>
       </c>
@@ -15294,7 +15291,7 @@
         <v>update lab set lab = 'Argonne National Laboratory', country = '' where lab_id = 460</v>
       </c>
     </row>
-    <row r="460" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="460" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A460">
         <v>461</v>
       </c>
@@ -15318,7 +15315,7 @@
         <v>update lab set lab = 'State University of New York - Marine Sciences Research Center', country = '' where lab_id = 461</v>
       </c>
     </row>
-    <row r="461" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="461" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A461">
         <v>462</v>
       </c>
@@ -15342,7 +15339,7 @@
         <v>update lab set lab = 'HCMR Hellenic Centre for Marine Research', country = '' where lab_id = 462</v>
       </c>
     </row>
-    <row r="462" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="462" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A462">
         <v>463</v>
       </c>
@@ -15363,7 +15360,7 @@
         <v>update lab set lab = 'Malaysian Nuclear Agency', country = '' where lab_id = 463</v>
       </c>
     </row>
-    <row r="463" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="463" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A463">
         <v>464</v>
       </c>
@@ -15387,7 +15384,7 @@
         <v>update lab set lab = 'Marine Radioecology Group - Center for Radiation Safety Technology and Metrology - National Nuclear Energy Agency of Indonesia (BATAN)', country = '' where lab_id = 464</v>
       </c>
     </row>
-    <row r="464" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="464" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A464">
         <v>465</v>
       </c>
@@ -15408,7 +15405,7 @@
         <v>update lab set lab = 'Fukushima University', country = '' where lab_id = 465</v>
       </c>
     </row>
-    <row r="465" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="465" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A465">
         <v>466</v>
       </c>
@@ -15432,7 +15429,7 @@
         <v>update lab set lab = 'State University of Novi Pazar', country = '' where lab_id = 466</v>
       </c>
     </row>
-    <row r="466" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="466" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A466">
         <v>467</v>
       </c>
@@ -15453,7 +15450,7 @@
         <v>update lab set lab = 'Laboratoire d'Etude et de Suivi  de l'Environnement', country = '' where lab_id = 467</v>
       </c>
     </row>
-    <row r="467" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="467" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A467">
         <v>468</v>
       </c>
@@ -15474,7 +15471,7 @@
         <v>update lab set lab = 'Korea Institute of Ocean Science &amp; Technology', country = '' where lab_id = 468</v>
       </c>
     </row>
-    <row r="468" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="468" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A468">
         <v>469</v>
       </c>
@@ -15495,7 +15492,7 @@
         <v>update lab set lab = 'Universiti Kebangsaan Malaysia', country = '' where lab_id = 469</v>
       </c>
     </row>
-    <row r="469" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="469" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A469">
         <v>470</v>
       </c>
@@ -15519,7 +15516,7 @@
         <v>update lab set lab = 'Ongkarak Nuclear Research Center - Thailand Institute of Nuclear Technology', country = '' where lab_id = 470</v>
       </c>
     </row>
-    <row r="470" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="470" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A470">
         <v>471</v>
       </c>
@@ -15540,7 +15537,7 @@
         <v>update lab set lab = 'Department of Physics - Universidad de Las Palmas de Gran Canaria', country = '' where lab_id = 471</v>
       </c>
     </row>
-    <row r="471" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="471" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A471">
         <v>472</v>
       </c>
@@ -15564,7 +15561,7 @@
         <v>update lab set lab = 'Department of Chemistry - Simon Fraser University', country = '' where lab_id = 472</v>
       </c>
     </row>
-    <row r="472" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="472" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A472">
         <v>473</v>
       </c>
@@ -15588,7 +15585,7 @@
         <v>update lab set lab = 'Iryo Sosei University (former Iwaki Meisei University)', country = '' where lab_id = 473</v>
       </c>
     </row>
-    <row r="473" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="473" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A473">
         <v>474</v>
       </c>
@@ -15609,7 +15606,7 @@
         <v>update lab set lab = 'Kobe University', country = '' where lab_id = 474</v>
       </c>
     </row>
-    <row r="474" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="474" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A474">
         <v>475</v>
       </c>
@@ -15633,7 +15630,7 @@
         <v>update lab set lab = 'Mutsu Establishment - Japan Atomic Energy Agency', country = '' where lab_id = 475</v>
       </c>
     </row>
-    <row r="475" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="475" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A475">
         <v>476</v>
       </c>
@@ -15654,7 +15651,7 @@
         <v>update lab set lab = 'Niigata Prefectural Institute of Environmental Radiation Monitoring', country = '' where lab_id = 476</v>
       </c>
     </row>
-    <row r="476" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="476" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A476">
         <v>477</v>
       </c>
@@ -15675,7 +15672,7 @@
         <v>update lab set lab = 'Miyagi Prefecture Environmental Radiation Monitoring Center (former Environmental Radioactivity Research Institute of Miyagi)', country = '' where lab_id = 477</v>
       </c>
     </row>
-    <row r="477" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="477" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A477">
         <v>478</v>
       </c>
@@ -15696,7 +15693,7 @@
         <v>update lab set lab = 'Faculty of Engineering - Hokkaido University', country = '' where lab_id = 478</v>
       </c>
     </row>
-    <row r="478" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="478" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A478">
         <v>479</v>
       </c>
@@ -15717,7 +15714,7 @@
         <v>update lab set lab = 'Fukushima Agricultural Technology Centre', country = '' where lab_id = 479</v>
       </c>
     </row>
-    <row r="479" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="479" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A479">
         <v>480</v>
       </c>
@@ -15741,7 +15738,7 @@
         <v>update lab set lab = 'National Research Institute of Fisheries Science (former Tokai Regional Fisheries Research Laboratory), Japan Fisheries Research and Education Agency', country = '' where lab_id = 480</v>
       </c>
     </row>
-    <row r="480" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="480" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A480">
         <v>481</v>
       </c>
@@ -15765,7 +15762,7 @@
         <v>update lab set lab = 'Japan Fisheries Research and Education Agency (former Fisheries Research Agency, and National Fisheries University)', country = '' where lab_id = 481</v>
       </c>
     </row>
-    <row r="481" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="481" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A481">
         <v>482</v>
       </c>
@@ -15789,7 +15786,7 @@
         <v>update lab set lab = 'National Institute of Radiological Sciences', country = '' where lab_id = 482</v>
       </c>
     </row>
-    <row r="482" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="482" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A482">
         <v>483</v>
       </c>
@@ -15810,7 +15807,7 @@
         <v>update lab set lab = 'Fukushima Prefectural Fisheries Experimental Station', country = '' where lab_id = 483</v>
       </c>
     </row>
-    <row r="483" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="483" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A483">
         <v>484</v>
       </c>
@@ -15834,7 +15831,7 @@
         <v>update lab set lab = 'Universidade Federal Fluminense - InInstituto de Biologia', country = '' where lab_id = 484</v>
       </c>
     </row>
-    <row r="484" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="484" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A484">
         <v>485</v>
       </c>
@@ -15855,7 +15852,7 @@
         <v>update lab set lab = 'Sudan Atomic Energy Commission', country = '' where lab_id = 485</v>
       </c>
     </row>
-    <row r="485" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="485" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A485">
         <v>486</v>
       </c>
@@ -15873,7 +15870,7 @@
         <v>update lab set lab = 'Duy Tan University - Institute of Research and Development', country = '' where lab_id = 486</v>
       </c>
     </row>
-    <row r="486" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="486" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A486">
         <v>487</v>
       </c>
@@ -15894,7 +15891,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire - Laboratoire de Radioécologie de Cherbourg-Octeville', country = '' where lab_id = 487</v>
       </c>
     </row>
-    <row r="487" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="487" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A487">
         <v>488</v>
       </c>
@@ -15912,7 +15909,7 @@
         <v>update lab set lab = 'University of the Faroe Islands', country = '' where lab_id = 488</v>
       </c>
     </row>
-    <row r="488" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="488" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A488">
         <v>489</v>
       </c>
@@ -15933,7 +15930,7 @@
         <v>update lab set lab = 'Norwegian University of Science and Technology - Department of Biology', country = '' where lab_id = 489</v>
       </c>
     </row>
-    <row r="489" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="489" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A489">
         <v>490</v>
       </c>
@@ -15954,7 +15951,7 @@
         <v>update lab set lab = 'University of Gothenburg - Department of Biological and Environmental Sciences', country = '' where lab_id = 490</v>
       </c>
     </row>
-    <row r="490" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="490" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A490">
         <v>491</v>
       </c>
@@ -15975,7 +15972,7 @@
         <v>update lab set lab = 'Risø National Laboratory', country = '' where lab_id = 491</v>
       </c>
     </row>
-    <row r="491" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="491" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A491">
         <v>492</v>
       </c>
@@ -15996,7 +15993,7 @@
         <v>update lab set lab = 'Urbino University - Institute of General Chemistry', country = '' where lab_id = 492</v>
       </c>
     </row>
-    <row r="492" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="492" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A492">
         <v>493</v>
       </c>
@@ -16014,7 +16011,7 @@
         <v>update lab set lab = 'University of Gdańsk - Faculty of Chemistry', country = '' where lab_id = 493</v>
       </c>
     </row>
-    <row r="493" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="493" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A493">
         <v>494</v>
       </c>
@@ -16035,7 +16032,7 @@
         <v>update lab set lab = 'University of Otago - Department of Chemistry', country = '' where lab_id = 494</v>
       </c>
     </row>
-    <row r="494" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="494" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A494">
         <v>495</v>
       </c>
@@ -16056,7 +16053,7 @@
         <v>update lab set lab = 'University of Silesia - Institute of Physics', country = '' where lab_id = 495</v>
       </c>
     </row>
-    <row r="495" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="495" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A495">
         <v>496</v>
       </c>
@@ -16071,7 +16068,7 @@
         <v>update lab set lab = 'Centro Nacional de Aceleradores (CNA), Universidad de Sevilla, Spain', country = '' where lab_id = 496</v>
       </c>
     </row>
-    <row r="496" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="496" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A496">
         <v>497</v>
       </c>
@@ -16086,7 +16083,7 @@
         <v>update lab set lab = 'Universidad de Sevilla, Spain', country = '' where lab_id = 497</v>
       </c>
     </row>
-    <row r="497" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="497" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A497">
         <v>498</v>
       </c>
@@ -16101,7 +16098,7 @@
         <v>update lab set lab = 'DTU Environment', country = '' where lab_id = 498</v>
       </c>
     </row>
-    <row r="498" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="498" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A498">
         <v>499</v>
       </c>
@@ -16119,7 +16116,7 @@
         <v>update lab set lab = 'Norwegian Radiation and Nuclear Safety Authority', country = '' where lab_id = 499</v>
       </c>
     </row>
-    <row r="499" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="499" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A499">
         <v>500</v>
       </c>
@@ -16137,7 +16134,7 @@
         <v>update lab set lab = 'Institut de Radioprotection et de Sûreté Nucléaire : LSE/SAME (ALOKA)', country = '' where lab_id = 500</v>
       </c>
     </row>
-    <row r="500" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="500" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A500">
         <v>501</v>
       </c>
@@ -16155,7 +16152,7 @@
         <v>update lab set lab = 'Sellafield Ltd', country = '' where lab_id = 501</v>
       </c>
     </row>
-    <row r="501" spans="1:14" x14ac:dyDescent="0.2">
+    <row r="501" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A501">
         <v>502</v>
       </c>
@@ -16169,7 +16166,7 @@
         <v>293</v>
       </c>
     </row>
-    <row r="502" spans="1:14" ht="16" x14ac:dyDescent="0.2">
+    <row r="502" spans="1:14" x14ac:dyDescent="0.25">
       <c r="A502">
         <v>503</v>
       </c>
@@ -16184,19 +16181,21 @@
       </c>
     </row>
   </sheetData>
-  <autoFilter ref="A1:K519" xr:uid="{2F13C8FC-6782-480C-9C4E-5575F36CC8BE}"/>
+  <autoFilter ref="A1:K519"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f3c01d95-e195-4940-9fb4-afa395d98e0b">
+      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    </lcf76f155ced4ddcb4097134ff3c332f>
+    <TaxCatchAll xmlns="77012c7d-7b27-41e5-8843-0f8877a4d830" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -16435,20 +16434,21 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <lcf76f155ced4ddcb4097134ff3c332f xmlns="f3c01d95-e195-4940-9fb4-afa395d98e0b">
-      <Terms xmlns="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    </lcf76f155ced4ddcb4097134ff3c332f>
-    <TaxCatchAll xmlns="77012c7d-7b27-41e5-8843-0f8877a4d830" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70630E28-52C0-4D0E-9782-67C868EE0408}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA1F0F8-DC4D-4181-A3DE-03D28F858DC2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
+    <ds:schemaRef ds:uri="77012c7d-7b27-41e5-8843-0f8877a4d830"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -16473,12 +16473,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{8CA1F0F8-DC4D-4181-A3DE-03D28F858DC2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{70630E28-52C0-4D0E-9782-67C868EE0408}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="f3c01d95-e195-4940-9fb4-afa395d98e0b"/>
-    <ds:schemaRef ds:uri="77012c7d-7b27-41e5-8843-0f8877a4d830"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>